<commit_message>
Adds More MacBook Information
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -5,22 +5,35 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Triviali Configuration Program\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Triviali Configuration Program\Triviali Configuration Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6282DB92-0859-4A25-B6C6-BB649BCABDA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCEEA63B-D0FD-4374-94F8-14E551EFBFAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1872" uniqueCount="423">
   <si>
     <t>make</t>
   </si>
@@ -644,24 +657,664 @@
   </si>
   <si>
     <t>Win11 22H2</t>
+  </si>
+  <si>
+    <t>A2681</t>
+  </si>
+  <si>
+    <t>A2779</t>
+  </si>
+  <si>
+    <t>M2 8 CORE CPU</t>
+  </si>
+  <si>
+    <t>M2 PRO 10-CORE</t>
+  </si>
+  <si>
+    <t>3.50GHZ      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.49GHZ       </t>
+  </si>
+  <si>
+    <t>16GB         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">32GB          </t>
+  </si>
+  <si>
+    <t>SSD          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD           </t>
+  </si>
+  <si>
+    <t>256GB        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">512GB         </t>
+  </si>
+  <si>
+    <t>NO OPTICAL   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO OPTICAL    </t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YES           </t>
+  </si>
+  <si>
+    <t>M2 8 CORE GPU</t>
+  </si>
+  <si>
+    <t>M2 PRO 16-CORE</t>
+  </si>
+  <si>
+    <t>16GB        </t>
+  </si>
+  <si>
+    <t>2560x1664</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3024X1964     </t>
+  </si>
+  <si>
+    <t>500 NITS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000 NITS     </t>
+  </si>
+  <si>
+    <t>NONTOUCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NONTOUCH      </t>
+  </si>
+  <si>
+    <t>13" M2 Air</t>
+  </si>
+  <si>
+    <t>14" M2 Pro</t>
+  </si>
+  <si>
+    <t>M2 Air</t>
+  </si>
+  <si>
+    <t>M2 Pro 14</t>
+  </si>
+  <si>
+    <t>3.20GHZ</t>
+  </si>
+  <si>
+    <t>SSD</t>
+  </si>
+  <si>
+    <t>2TB</t>
+  </si>
+  <si>
+    <t>NO OPTICAL</t>
+  </si>
+  <si>
+    <t>1000 NITS</t>
+  </si>
+  <si>
+    <t>32GB</t>
+  </si>
+  <si>
+    <t>1TB</t>
+  </si>
+  <si>
+    <t>512GB</t>
+  </si>
+  <si>
+    <t>A2442</t>
+  </si>
+  <si>
+    <t>M1 CHIP 8 CORE</t>
+  </si>
+  <si>
+    <t>M1 14 CORE GPU</t>
+  </si>
+  <si>
+    <t>3024x1964</t>
+  </si>
+  <si>
+    <t>A2337(Q6LR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.20GHZ       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">16GB          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">256GB         </t>
+  </si>
+  <si>
+    <t>M1 7 CORE GPU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16GB         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2560X1600    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">400 NITS     </t>
+  </si>
+  <si>
+    <t>A2251(ML85)</t>
+  </si>
+  <si>
+    <t>A2289(P3XY)</t>
+  </si>
+  <si>
+    <t>i7-1068NG7</t>
+  </si>
+  <si>
+    <t>i5-8257U</t>
+  </si>
+  <si>
+    <t>2.30GHZ</t>
+  </si>
+  <si>
+    <t>1.40GHZ</t>
+  </si>
+  <si>
+    <t>8GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSD      </t>
+  </si>
+  <si>
+    <t>256GB</t>
+  </si>
+  <si>
+    <t>IRISPLUSGRAPHIC</t>
+  </si>
+  <si>
+    <t>IRIS PLUS 645</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1536MB         </t>
+  </si>
+  <si>
+    <t>1536MB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2560X1600      </t>
+  </si>
+  <si>
+    <t>2560x1600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">500 NITS       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NONTOUCH </t>
+  </si>
+  <si>
+    <t>E20162</t>
+  </si>
+  <si>
+    <t>A2141(MD6P)</t>
+  </si>
+  <si>
+    <t>A2141(MD6Q)</t>
+  </si>
+  <si>
+    <t>A2141(MD6W)</t>
+  </si>
+  <si>
+    <t>A2179(MNHX)</t>
+  </si>
+  <si>
+    <t>i5-1030NG7</t>
+  </si>
+  <si>
+    <t>2.40GHZ</t>
+  </si>
+  <si>
+    <t>1.10GHz</t>
+  </si>
+  <si>
+    <t>4TB</t>
+  </si>
+  <si>
+    <t>RADEON PRO5300M</t>
+  </si>
+  <si>
+    <t>RADEON PRO5500M</t>
+  </si>
+  <si>
+    <t>4GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400 NITS       </t>
+  </si>
+  <si>
+    <t>L19161</t>
+  </si>
+  <si>
+    <t>M1891</t>
+  </si>
+  <si>
+    <t>A1990(LVDQ)</t>
+  </si>
+  <si>
+    <t>RADEON PRO560X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4GB           </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2880X1800     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">500 NITS      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NONTOUCH  </t>
+  </si>
+  <si>
+    <t>A1932(JK78)</t>
+  </si>
+  <si>
+    <t>i5-8210Y</t>
+  </si>
+  <si>
+    <t>1.60GHZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YES </t>
+  </si>
+  <si>
+    <t>UHDGRAPHICS 617</t>
+  </si>
+  <si>
+    <t>A1932(JK7M)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L1881  </t>
+  </si>
+  <si>
+    <t>A1989(JHD2)</t>
+  </si>
+  <si>
+    <t>i7-8559U</t>
+  </si>
+  <si>
+    <t>2.70GHZ</t>
+  </si>
+  <si>
+    <t>IRIS PLUS 655</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1536MB       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">500 NITS     </t>
+  </si>
+  <si>
+    <t>M18152</t>
+  </si>
+  <si>
+    <t>A1989(LVDL)</t>
+  </si>
+  <si>
+    <t>i7-8569U</t>
+  </si>
+  <si>
+    <t>2.80GHZ</t>
+  </si>
+  <si>
+    <t>A1989(LVDM)</t>
+  </si>
+  <si>
+    <t>A1990(LVCG)</t>
+  </si>
+  <si>
+    <t>I9-9880H</t>
+  </si>
+  <si>
+    <t>2880X1800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">500 NITS </t>
+  </si>
+  <si>
+    <t>A1990(LVDR)</t>
+  </si>
+  <si>
+    <t>2880x1800</t>
+  </si>
+  <si>
+    <t>A1990(JG5J)</t>
+  </si>
+  <si>
+    <t>m18151</t>
+  </si>
+  <si>
+    <t>A1990(JG5M)</t>
+  </si>
+  <si>
+    <t>A1932(LYWN)</t>
+  </si>
+  <si>
+    <t>A1989(JHC9)</t>
+  </si>
+  <si>
+    <t>I5-8259U</t>
+  </si>
+  <si>
+    <t>A1989(JHD3)</t>
+  </si>
+  <si>
+    <t>m18152</t>
+  </si>
+  <si>
+    <t>A1990(JGH6)</t>
+  </si>
+  <si>
+    <t>i9-8950HK</t>
+  </si>
+  <si>
+    <t>2.90GHZ</t>
+  </si>
+  <si>
+    <t>A1990(JGH8)</t>
+  </si>
+  <si>
+    <t>16GB or 32GB</t>
+  </si>
+  <si>
+    <t>A1706(GTDX)</t>
+  </si>
+  <si>
+    <t>i7-6567U</t>
+  </si>
+  <si>
+    <t>3.30GHz</t>
+  </si>
+  <si>
+    <t>IRISGRAPHICS550</t>
+  </si>
+  <si>
+    <t>A1707(GTFM)</t>
+  </si>
+  <si>
+    <t>i7-6820HQ</t>
+  </si>
+  <si>
+    <t>RADEON PRO455</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2GB          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2880X1800    </t>
+  </si>
+  <si>
+    <t>L16133</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A1706(HV2L)  </t>
+  </si>
+  <si>
+    <t>i5-7267U</t>
+  </si>
+  <si>
+    <t>3.10GHZ</t>
+  </si>
+  <si>
+    <t>IRIS PLUS 650</t>
+  </si>
+  <si>
+    <t>A1707(HTDF)</t>
+  </si>
+  <si>
+    <t>i7-7920HQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.10GHZ </t>
+  </si>
+  <si>
+    <t>RADEON PRO560</t>
+  </si>
+  <si>
+    <t>A1707(HTD6)</t>
+  </si>
+  <si>
+    <t>I7-7820HQ</t>
+  </si>
+  <si>
+    <t>2.90GHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4GB          </t>
+  </si>
+  <si>
+    <t>M17143</t>
+  </si>
+  <si>
+    <t>A1707(H040)</t>
+  </si>
+  <si>
+    <t>i7-6920HQ</t>
+  </si>
+  <si>
+    <t>RADEON PRO460</t>
+  </si>
+  <si>
+    <t>A1707(HTDD)</t>
+  </si>
+  <si>
+    <t>i7-7700HQ</t>
+  </si>
+  <si>
+    <t>RADEON PRO555</t>
+  </si>
+  <si>
+    <t>2GB</t>
+  </si>
+  <si>
+    <t>A1707(H03Q)</t>
+  </si>
+  <si>
+    <t>I7-6820HQ</t>
+  </si>
+  <si>
+    <t>A1706(GYFH)</t>
+  </si>
+  <si>
+    <t>I5-6267U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NONTOUCH       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">L16132  </t>
+  </si>
+  <si>
+    <t>A1706(HV2R)</t>
+  </si>
+  <si>
+    <t>i7-7567U</t>
+  </si>
+  <si>
+    <t>3.50GHz</t>
+  </si>
+  <si>
+    <t>512GB or 1TB</t>
+  </si>
+  <si>
+    <t>m17142</t>
+  </si>
+  <si>
+    <t>A1707(GTF1)</t>
+  </si>
+  <si>
+    <t>A1706(GTFJ)</t>
+  </si>
+  <si>
+    <t>i5-6267U</t>
+  </si>
+  <si>
+    <t>L16132</t>
+  </si>
+  <si>
+    <t>A1706(HV2Q)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i5-7267U     </t>
+  </si>
+  <si>
+    <t>M14111</t>
+  </si>
+  <si>
+    <t>E15121</t>
+  </si>
+  <si>
+    <t>300 NITS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">400 NITS      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">300 NITS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">300 NITS       </t>
+  </si>
+  <si>
+    <t>2304x1440</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2304X1440     </t>
+  </si>
+  <si>
+    <t>2560X1600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1536MB        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1536MB   </t>
+  </si>
+  <si>
+    <t>IRIS</t>
+  </si>
+  <si>
+    <t>HDGRAPHICS 5300</t>
+  </si>
+  <si>
+    <t>HDGRAPHICS 615</t>
+  </si>
+  <si>
+    <t>IRISGRAPHIC6100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IRIS     </t>
+  </si>
+  <si>
+    <t>128GB</t>
+  </si>
+  <si>
+    <t>1.20GHZ</t>
+  </si>
+  <si>
+    <t>3.00GHZ</t>
+  </si>
+  <si>
+    <t>2.70GHz</t>
+  </si>
+  <si>
+    <t>i5-4258U</t>
+  </si>
+  <si>
+    <t>i5-4278U</t>
+  </si>
+  <si>
+    <t>M-5Y71</t>
+  </si>
+  <si>
+    <t>i5-7Y54</t>
+  </si>
+  <si>
+    <t>i7-5557U</t>
+  </si>
+  <si>
+    <t>i7-4578U</t>
+  </si>
+  <si>
+    <t>i5-4308U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i5-5287U </t>
+  </si>
+  <si>
+    <t>i5-5257U</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i5-5257U </t>
+  </si>
+  <si>
+    <t>A1502(FGYY)</t>
+  </si>
+  <si>
+    <t>A1502(G3QH)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A1534(GCN2) </t>
+  </si>
+  <si>
+    <t>A1534(HH22)</t>
+  </si>
+  <si>
+    <t>A1502(FVH8)</t>
+  </si>
+  <si>
+    <t>A1502(G3QR)</t>
+  </si>
+  <si>
+    <t>A1502(G3QT)</t>
+  </si>
+  <si>
+    <t>A1502(G3QJ)</t>
+  </si>
+  <si>
+    <t>A1502(FVH7)</t>
+  </si>
+  <si>
+    <t>A1502(FVH6)</t>
+  </si>
+  <si>
+    <t>A1502(FVH5)</t>
+  </si>
+  <si>
+    <t>M1  Pro 14</t>
+  </si>
+  <si>
+    <t>M1 Air 13</t>
+  </si>
+  <si>
+    <t>Intel Pro 13</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -672,7 +1325,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -680,30 +1333,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1006,95 +1641,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y30"/>
+  <dimension ref="A1:Y80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="Y65" sqref="Y65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="23.21875" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
     <col min="14" max="14" width="15.6640625" customWidth="1"/>
+    <col min="18" max="18" width="16" customWidth="1"/>
+    <col min="22" max="22" width="12" customWidth="1"/>
     <col min="24" max="24" width="18.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2540,7 +3177,7 @@
         <v>140</v>
       </c>
       <c r="S20" t="s">
-        <v>48</v>
+        <v>215</v>
       </c>
       <c r="T20" t="s">
         <v>141</v>
@@ -2617,7 +3254,7 @@
         <v>140</v>
       </c>
       <c r="S21" t="s">
-        <v>48</v>
+        <v>215</v>
       </c>
       <c r="T21" t="s">
         <v>141</v>
@@ -2694,7 +3331,7 @@
         <v>140</v>
       </c>
       <c r="S22" t="s">
-        <v>48</v>
+        <v>127</v>
       </c>
       <c r="T22" t="s">
         <v>141</v>
@@ -3329,6 +3966,3481 @@
       </c>
       <c r="Y30" t="s">
         <v>204</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" t="s">
+        <v>235</v>
+      </c>
+      <c r="C31" t="s">
+        <v>208</v>
+      </c>
+      <c r="D31" t="s">
+        <v>210</v>
+      </c>
+      <c r="E31" t="s">
+        <v>212</v>
+      </c>
+      <c r="F31" t="s">
+        <v>214</v>
+      </c>
+      <c r="G31" t="s">
+        <v>216</v>
+      </c>
+      <c r="H31" t="s">
+        <v>218</v>
+      </c>
+      <c r="I31" t="s">
+        <v>220</v>
+      </c>
+      <c r="J31" t="s">
+        <v>222</v>
+      </c>
+      <c r="K31" t="s">
+        <v>155</v>
+      </c>
+      <c r="L31" t="s">
+        <v>35</v>
+      </c>
+      <c r="M31" t="s">
+        <v>35</v>
+      </c>
+      <c r="N31" t="s">
+        <v>36</v>
+      </c>
+      <c r="O31" t="s">
+        <v>37</v>
+      </c>
+      <c r="P31" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>139</v>
+      </c>
+      <c r="R31" t="s">
+        <v>224</v>
+      </c>
+      <c r="S31" t="s">
+        <v>226</v>
+      </c>
+      <c r="T31" t="s">
+        <v>227</v>
+      </c>
+      <c r="U31" t="s">
+        <v>229</v>
+      </c>
+      <c r="V31" t="s">
+        <v>231</v>
+      </c>
+      <c r="W31" t="s">
+        <v>44</v>
+      </c>
+      <c r="X31" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>113</v>
+      </c>
+      <c r="B32" t="s">
+        <v>236</v>
+      </c>
+      <c r="C32" t="s">
+        <v>209</v>
+      </c>
+      <c r="D32" t="s">
+        <v>211</v>
+      </c>
+      <c r="E32" t="s">
+        <v>213</v>
+      </c>
+      <c r="F32" t="s">
+        <v>215</v>
+      </c>
+      <c r="G32" t="s">
+        <v>217</v>
+      </c>
+      <c r="H32" t="s">
+        <v>219</v>
+      </c>
+      <c r="I32" t="s">
+        <v>221</v>
+      </c>
+      <c r="J32" t="s">
+        <v>223</v>
+      </c>
+      <c r="K32" t="s">
+        <v>155</v>
+      </c>
+      <c r="L32" t="s">
+        <v>35</v>
+      </c>
+      <c r="M32" t="s">
+        <v>35</v>
+      </c>
+      <c r="N32" t="s">
+        <v>36</v>
+      </c>
+      <c r="O32" t="s">
+        <v>37</v>
+      </c>
+      <c r="P32" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>139</v>
+      </c>
+      <c r="R32" t="s">
+        <v>225</v>
+      </c>
+      <c r="S32" t="s">
+        <v>215</v>
+      </c>
+      <c r="T32" t="s">
+        <v>228</v>
+      </c>
+      <c r="U32" t="s">
+        <v>230</v>
+      </c>
+      <c r="V32" t="s">
+        <v>232</v>
+      </c>
+      <c r="W32" t="s">
+        <v>44</v>
+      </c>
+      <c r="X32" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>113</v>
+      </c>
+      <c r="B33" t="s">
+        <v>420</v>
+      </c>
+      <c r="C33" t="s">
+        <v>245</v>
+      </c>
+      <c r="D33" t="s">
+        <v>246</v>
+      </c>
+      <c r="E33" t="s">
+        <v>237</v>
+      </c>
+      <c r="F33" t="s">
+        <v>137</v>
+      </c>
+      <c r="G33" t="s">
+        <v>238</v>
+      </c>
+      <c r="H33" t="s">
+        <v>244</v>
+      </c>
+      <c r="I33" t="s">
+        <v>240</v>
+      </c>
+      <c r="J33" t="s">
+        <v>222</v>
+      </c>
+      <c r="K33" t="s">
+        <v>155</v>
+      </c>
+      <c r="L33" t="s">
+        <v>35</v>
+      </c>
+      <c r="M33" t="s">
+        <v>35</v>
+      </c>
+      <c r="N33" t="s">
+        <v>36</v>
+      </c>
+      <c r="O33" t="s">
+        <v>37</v>
+      </c>
+      <c r="P33" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>139</v>
+      </c>
+      <c r="R33" t="s">
+        <v>247</v>
+      </c>
+      <c r="S33" t="s">
+        <v>137</v>
+      </c>
+      <c r="T33" t="s">
+        <v>248</v>
+      </c>
+      <c r="U33" t="s">
+        <v>241</v>
+      </c>
+      <c r="V33" t="s">
+        <v>231</v>
+      </c>
+      <c r="W33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>113</v>
+      </c>
+      <c r="B34" t="s">
+        <v>421</v>
+      </c>
+      <c r="C34" t="s">
+        <v>249</v>
+      </c>
+      <c r="D34" t="s">
+        <v>246</v>
+      </c>
+      <c r="E34" t="s">
+        <v>250</v>
+      </c>
+      <c r="F34" t="s">
+        <v>251</v>
+      </c>
+      <c r="G34" t="s">
+        <v>217</v>
+      </c>
+      <c r="H34" t="s">
+        <v>252</v>
+      </c>
+      <c r="I34" t="s">
+        <v>221</v>
+      </c>
+      <c r="J34" t="s">
+        <v>222</v>
+      </c>
+      <c r="K34" t="s">
+        <v>155</v>
+      </c>
+      <c r="L34" t="s">
+        <v>35</v>
+      </c>
+      <c r="M34" t="s">
+        <v>35</v>
+      </c>
+      <c r="N34" t="s">
+        <v>36</v>
+      </c>
+      <c r="O34" t="s">
+        <v>37</v>
+      </c>
+      <c r="P34" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>139</v>
+      </c>
+      <c r="R34" t="s">
+        <v>253</v>
+      </c>
+      <c r="S34" t="s">
+        <v>254</v>
+      </c>
+      <c r="T34" t="s">
+        <v>255</v>
+      </c>
+      <c r="U34" t="s">
+        <v>256</v>
+      </c>
+      <c r="V34" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35" t="s">
+        <v>422</v>
+      </c>
+      <c r="C35" t="s">
+        <v>257</v>
+      </c>
+      <c r="D35" t="s">
+        <v>259</v>
+      </c>
+      <c r="E35" t="s">
+        <v>261</v>
+      </c>
+      <c r="F35" t="s">
+        <v>242</v>
+      </c>
+      <c r="G35" t="s">
+        <v>238</v>
+      </c>
+      <c r="H35" t="s">
+        <v>244</v>
+      </c>
+      <c r="I35" t="s">
+        <v>240</v>
+      </c>
+      <c r="J35" t="s">
+        <v>222</v>
+      </c>
+      <c r="K35" t="s">
+        <v>155</v>
+      </c>
+      <c r="L35" t="s">
+        <v>35</v>
+      </c>
+      <c r="M35" t="s">
+        <v>35</v>
+      </c>
+      <c r="N35" t="s">
+        <v>36</v>
+      </c>
+      <c r="O35" t="s">
+        <v>37</v>
+      </c>
+      <c r="P35" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>38</v>
+      </c>
+      <c r="R35" t="s">
+        <v>266</v>
+      </c>
+      <c r="S35" t="s">
+        <v>268</v>
+      </c>
+      <c r="T35" t="s">
+        <v>270</v>
+      </c>
+      <c r="U35" t="s">
+        <v>272</v>
+      </c>
+      <c r="V35" t="s">
+        <v>273</v>
+      </c>
+      <c r="W35" t="s">
+        <v>274</v>
+      </c>
+      <c r="X35" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>113</v>
+      </c>
+      <c r="C36" t="s">
+        <v>258</v>
+      </c>
+      <c r="D36" t="s">
+        <v>260</v>
+      </c>
+      <c r="E36" t="s">
+        <v>262</v>
+      </c>
+      <c r="F36" t="s">
+        <v>263</v>
+      </c>
+      <c r="G36" t="s">
+        <v>264</v>
+      </c>
+      <c r="H36" t="s">
+        <v>265</v>
+      </c>
+      <c r="I36" t="s">
+        <v>240</v>
+      </c>
+      <c r="J36" t="s">
+        <v>222</v>
+      </c>
+      <c r="K36" t="s">
+        <v>155</v>
+      </c>
+      <c r="L36" t="s">
+        <v>35</v>
+      </c>
+      <c r="M36" t="s">
+        <v>35</v>
+      </c>
+      <c r="N36" t="s">
+        <v>36</v>
+      </c>
+      <c r="O36" t="s">
+        <v>37</v>
+      </c>
+      <c r="P36" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>38</v>
+      </c>
+      <c r="R36" t="s">
+        <v>267</v>
+      </c>
+      <c r="S36" t="s">
+        <v>269</v>
+      </c>
+      <c r="T36" t="s">
+        <v>271</v>
+      </c>
+      <c r="U36" t="s">
+        <v>229</v>
+      </c>
+      <c r="V36" t="s">
+        <v>231</v>
+      </c>
+      <c r="X36" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>113</v>
+      </c>
+      <c r="C37" t="s">
+        <v>275</v>
+      </c>
+      <c r="D37" t="s">
+        <v>162</v>
+      </c>
+      <c r="E37" t="s">
+        <v>154</v>
+      </c>
+      <c r="F37" t="s">
+        <v>137</v>
+      </c>
+      <c r="G37" t="s">
+        <v>238</v>
+      </c>
+      <c r="H37" t="s">
+        <v>244</v>
+      </c>
+      <c r="I37" t="s">
+        <v>240</v>
+      </c>
+      <c r="J37" t="s">
+        <v>222</v>
+      </c>
+      <c r="K37" t="s">
+        <v>155</v>
+      </c>
+      <c r="L37" t="s">
+        <v>35</v>
+      </c>
+      <c r="M37" t="s">
+        <v>35</v>
+      </c>
+      <c r="N37" t="s">
+        <v>36</v>
+      </c>
+      <c r="O37" t="s">
+        <v>37</v>
+      </c>
+      <c r="P37" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>117</v>
+      </c>
+      <c r="R37" t="s">
+        <v>283</v>
+      </c>
+      <c r="S37" t="s">
+        <v>285</v>
+      </c>
+      <c r="T37" t="s">
+        <v>120</v>
+      </c>
+      <c r="U37" t="s">
+        <v>229</v>
+      </c>
+      <c r="V37" t="s">
+        <v>273</v>
+      </c>
+      <c r="W37" t="s">
+        <v>287</v>
+      </c>
+      <c r="X37" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38" t="s">
+        <v>276</v>
+      </c>
+      <c r="D38" t="s">
+        <v>125</v>
+      </c>
+      <c r="E38" t="s">
+        <v>261</v>
+      </c>
+      <c r="F38" t="s">
+        <v>137</v>
+      </c>
+      <c r="G38" t="s">
+        <v>238</v>
+      </c>
+      <c r="H38" t="s">
+        <v>243</v>
+      </c>
+      <c r="I38" t="s">
+        <v>240</v>
+      </c>
+      <c r="J38" t="s">
+        <v>222</v>
+      </c>
+      <c r="K38" t="s">
+        <v>155</v>
+      </c>
+      <c r="L38" t="s">
+        <v>35</v>
+      </c>
+      <c r="M38" t="s">
+        <v>35</v>
+      </c>
+      <c r="N38" t="s">
+        <v>36</v>
+      </c>
+      <c r="O38" t="s">
+        <v>37</v>
+      </c>
+      <c r="P38" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>117</v>
+      </c>
+      <c r="R38" t="s">
+        <v>284</v>
+      </c>
+      <c r="S38" t="s">
+        <v>285</v>
+      </c>
+      <c r="T38" t="s">
+        <v>120</v>
+      </c>
+      <c r="U38" t="s">
+        <v>229</v>
+      </c>
+      <c r="V38" t="s">
+        <v>273</v>
+      </c>
+      <c r="W38" t="s">
+        <v>287</v>
+      </c>
+      <c r="X38" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" t="s">
+        <v>277</v>
+      </c>
+      <c r="D39" t="s">
+        <v>125</v>
+      </c>
+      <c r="E39" t="s">
+        <v>261</v>
+      </c>
+      <c r="F39" t="s">
+        <v>242</v>
+      </c>
+      <c r="G39" t="s">
+        <v>238</v>
+      </c>
+      <c r="H39" t="s">
+        <v>282</v>
+      </c>
+      <c r="I39" t="s">
+        <v>240</v>
+      </c>
+      <c r="J39" t="s">
+        <v>222</v>
+      </c>
+      <c r="K39" t="s">
+        <v>155</v>
+      </c>
+      <c r="L39" t="s">
+        <v>35</v>
+      </c>
+      <c r="M39" t="s">
+        <v>35</v>
+      </c>
+      <c r="N39" t="s">
+        <v>36</v>
+      </c>
+      <c r="O39" t="s">
+        <v>37</v>
+      </c>
+      <c r="P39" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>117</v>
+      </c>
+      <c r="R39" t="s">
+        <v>284</v>
+      </c>
+      <c r="S39" t="s">
+        <v>263</v>
+      </c>
+      <c r="T39" t="s">
+        <v>120</v>
+      </c>
+      <c r="U39" t="s">
+        <v>229</v>
+      </c>
+      <c r="V39" t="s">
+        <v>231</v>
+      </c>
+      <c r="W39" t="s">
+        <v>287</v>
+      </c>
+      <c r="X39" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>113</v>
+      </c>
+      <c r="C40" t="s">
+        <v>278</v>
+      </c>
+      <c r="D40" t="s">
+        <v>279</v>
+      </c>
+      <c r="E40" t="s">
+        <v>281</v>
+      </c>
+      <c r="F40" t="s">
+        <v>137</v>
+      </c>
+      <c r="G40" t="s">
+        <v>238</v>
+      </c>
+      <c r="H40" t="s">
+        <v>265</v>
+      </c>
+      <c r="I40" t="s">
+        <v>240</v>
+      </c>
+      <c r="J40" t="s">
+        <v>222</v>
+      </c>
+      <c r="K40" t="s">
+        <v>155</v>
+      </c>
+      <c r="L40" t="s">
+        <v>35</v>
+      </c>
+      <c r="M40" t="s">
+        <v>35</v>
+      </c>
+      <c r="N40" t="s">
+        <v>36</v>
+      </c>
+      <c r="O40" t="s">
+        <v>37</v>
+      </c>
+      <c r="P40" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>38</v>
+      </c>
+      <c r="R40" t="s">
+        <v>266</v>
+      </c>
+      <c r="S40" t="s">
+        <v>268</v>
+      </c>
+      <c r="T40" t="s">
+        <v>270</v>
+      </c>
+      <c r="U40" t="s">
+        <v>286</v>
+      </c>
+      <c r="V40" t="s">
+        <v>273</v>
+      </c>
+      <c r="W40" t="s">
+        <v>288</v>
+      </c>
+      <c r="X40" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>113</v>
+      </c>
+      <c r="C41" t="s">
+        <v>289</v>
+      </c>
+      <c r="D41" t="s">
+        <v>162</v>
+      </c>
+      <c r="E41" t="s">
+        <v>98</v>
+      </c>
+      <c r="F41" t="s">
+        <v>53</v>
+      </c>
+      <c r="G41" t="s">
+        <v>238</v>
+      </c>
+      <c r="H41" t="s">
+        <v>244</v>
+      </c>
+      <c r="I41" t="s">
+        <v>240</v>
+      </c>
+      <c r="J41" t="s">
+        <v>222</v>
+      </c>
+      <c r="K41" t="s">
+        <v>155</v>
+      </c>
+      <c r="L41" t="s">
+        <v>35</v>
+      </c>
+      <c r="M41" t="s">
+        <v>35</v>
+      </c>
+      <c r="N41" t="s">
+        <v>36</v>
+      </c>
+      <c r="O41" t="s">
+        <v>37</v>
+      </c>
+      <c r="P41" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>117</v>
+      </c>
+      <c r="R41" t="s">
+        <v>290</v>
+      </c>
+      <c r="S41" t="s">
+        <v>291</v>
+      </c>
+      <c r="T41" t="s">
+        <v>292</v>
+      </c>
+      <c r="U41" t="s">
+        <v>293</v>
+      </c>
+      <c r="V41" t="s">
+        <v>294</v>
+      </c>
+      <c r="X41" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>113</v>
+      </c>
+      <c r="C42" t="s">
+        <v>295</v>
+      </c>
+      <c r="D42" t="s">
+        <v>296</v>
+      </c>
+      <c r="E42" t="s">
+        <v>297</v>
+      </c>
+      <c r="F42" t="s">
+        <v>263</v>
+      </c>
+      <c r="G42" t="s">
+        <v>238</v>
+      </c>
+      <c r="H42" t="s">
+        <v>265</v>
+      </c>
+      <c r="I42" t="s">
+        <v>240</v>
+      </c>
+      <c r="J42" t="s">
+        <v>298</v>
+      </c>
+      <c r="K42" t="s">
+        <v>155</v>
+      </c>
+      <c r="L42" t="s">
+        <v>35</v>
+      </c>
+      <c r="M42" t="s">
+        <v>35</v>
+      </c>
+      <c r="N42" t="s">
+        <v>36</v>
+      </c>
+      <c r="O42" t="s">
+        <v>37</v>
+      </c>
+      <c r="P42" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>38</v>
+      </c>
+      <c r="R42" t="s">
+        <v>299</v>
+      </c>
+      <c r="S42" t="s">
+        <v>268</v>
+      </c>
+      <c r="T42" t="s">
+        <v>270</v>
+      </c>
+      <c r="U42" t="s">
+        <v>286</v>
+      </c>
+      <c r="V42" t="s">
+        <v>231</v>
+      </c>
+      <c r="X42" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>113</v>
+      </c>
+      <c r="C43" t="s">
+        <v>300</v>
+      </c>
+      <c r="D43" t="s">
+        <v>296</v>
+      </c>
+      <c r="E43" t="s">
+        <v>297</v>
+      </c>
+      <c r="F43" t="s">
+        <v>137</v>
+      </c>
+      <c r="G43" t="s">
+        <v>238</v>
+      </c>
+      <c r="H43" t="s">
+        <v>244</v>
+      </c>
+      <c r="I43" t="s">
+        <v>240</v>
+      </c>
+      <c r="J43" t="s">
+        <v>222</v>
+      </c>
+      <c r="K43" t="s">
+        <v>155</v>
+      </c>
+      <c r="L43" t="s">
+        <v>35</v>
+      </c>
+      <c r="M43" t="s">
+        <v>35</v>
+      </c>
+      <c r="N43" t="s">
+        <v>36</v>
+      </c>
+      <c r="O43" t="s">
+        <v>37</v>
+      </c>
+      <c r="P43" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>38</v>
+      </c>
+      <c r="R43" t="s">
+        <v>299</v>
+      </c>
+      <c r="S43" t="s">
+        <v>268</v>
+      </c>
+      <c r="T43" t="s">
+        <v>270</v>
+      </c>
+      <c r="U43" t="s">
+        <v>286</v>
+      </c>
+      <c r="V43" t="s">
+        <v>273</v>
+      </c>
+      <c r="W43" t="s">
+        <v>301</v>
+      </c>
+      <c r="X43" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>113</v>
+      </c>
+      <c r="C44" t="s">
+        <v>302</v>
+      </c>
+      <c r="D44" t="s">
+        <v>303</v>
+      </c>
+      <c r="E44" t="s">
+        <v>304</v>
+      </c>
+      <c r="F44" t="s">
+        <v>137</v>
+      </c>
+      <c r="G44" t="s">
+        <v>238</v>
+      </c>
+      <c r="H44" t="s">
+        <v>244</v>
+      </c>
+      <c r="I44" t="s">
+        <v>240</v>
+      </c>
+      <c r="J44" t="s">
+        <v>222</v>
+      </c>
+      <c r="K44" t="s">
+        <v>155</v>
+      </c>
+      <c r="L44" t="s">
+        <v>35</v>
+      </c>
+      <c r="M44" t="s">
+        <v>35</v>
+      </c>
+      <c r="N44" t="s">
+        <v>36</v>
+      </c>
+      <c r="O44" t="s">
+        <v>37</v>
+      </c>
+      <c r="P44" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>38</v>
+      </c>
+      <c r="R44" t="s">
+        <v>305</v>
+      </c>
+      <c r="S44" t="s">
+        <v>306</v>
+      </c>
+      <c r="T44" t="s">
+        <v>255</v>
+      </c>
+      <c r="U44" t="s">
+        <v>307</v>
+      </c>
+      <c r="V44" t="s">
+        <v>273</v>
+      </c>
+      <c r="W44" t="s">
+        <v>308</v>
+      </c>
+      <c r="X44" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>113</v>
+      </c>
+      <c r="C45" t="s">
+        <v>309</v>
+      </c>
+      <c r="D45" t="s">
+        <v>310</v>
+      </c>
+      <c r="E45" t="s">
+        <v>311</v>
+      </c>
+      <c r="F45" t="s">
+        <v>137</v>
+      </c>
+      <c r="G45" t="s">
+        <v>238</v>
+      </c>
+      <c r="H45" t="s">
+        <v>244</v>
+      </c>
+      <c r="I45" t="s">
+        <v>240</v>
+      </c>
+      <c r="J45" t="s">
+        <v>222</v>
+      </c>
+      <c r="K45" t="s">
+        <v>155</v>
+      </c>
+      <c r="L45" t="s">
+        <v>35</v>
+      </c>
+      <c r="M45" t="s">
+        <v>35</v>
+      </c>
+      <c r="N45" t="s">
+        <v>36</v>
+      </c>
+      <c r="O45" t="s">
+        <v>37</v>
+      </c>
+      <c r="P45" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>38</v>
+      </c>
+      <c r="R45" t="s">
+        <v>305</v>
+      </c>
+      <c r="S45" t="s">
+        <v>306</v>
+      </c>
+      <c r="T45" t="s">
+        <v>255</v>
+      </c>
+      <c r="U45" t="s">
+        <v>307</v>
+      </c>
+      <c r="V45" t="s">
+        <v>273</v>
+      </c>
+      <c r="X45" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>113</v>
+      </c>
+      <c r="C46" t="s">
+        <v>312</v>
+      </c>
+      <c r="D46" t="s">
+        <v>310</v>
+      </c>
+      <c r="E46" t="s">
+        <v>311</v>
+      </c>
+      <c r="F46" t="s">
+        <v>137</v>
+      </c>
+      <c r="G46" t="s">
+        <v>238</v>
+      </c>
+      <c r="H46" t="s">
+        <v>244</v>
+      </c>
+      <c r="I46" t="s">
+        <v>240</v>
+      </c>
+      <c r="J46" t="s">
+        <v>222</v>
+      </c>
+      <c r="K46" t="s">
+        <v>155</v>
+      </c>
+      <c r="L46" t="s">
+        <v>35</v>
+      </c>
+      <c r="M46" t="s">
+        <v>35</v>
+      </c>
+      <c r="N46" t="s">
+        <v>36</v>
+      </c>
+      <c r="O46" t="s">
+        <v>37</v>
+      </c>
+      <c r="P46" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>38</v>
+      </c>
+      <c r="R46" t="s">
+        <v>305</v>
+      </c>
+      <c r="S46" t="s">
+        <v>269</v>
+      </c>
+      <c r="T46" t="s">
+        <v>271</v>
+      </c>
+      <c r="U46" t="s">
+        <v>229</v>
+      </c>
+      <c r="V46" t="s">
+        <v>231</v>
+      </c>
+      <c r="X46" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>113</v>
+      </c>
+      <c r="C47" t="s">
+        <v>313</v>
+      </c>
+      <c r="D47" t="s">
+        <v>314</v>
+      </c>
+      <c r="E47" t="s">
+        <v>261</v>
+      </c>
+      <c r="F47" t="s">
+        <v>137</v>
+      </c>
+      <c r="G47" t="s">
+        <v>238</v>
+      </c>
+      <c r="H47" t="s">
+        <v>244</v>
+      </c>
+      <c r="I47" t="s">
+        <v>240</v>
+      </c>
+      <c r="J47" t="s">
+        <v>222</v>
+      </c>
+      <c r="K47" t="s">
+        <v>155</v>
+      </c>
+      <c r="L47" t="s">
+        <v>35</v>
+      </c>
+      <c r="M47" t="s">
+        <v>35</v>
+      </c>
+      <c r="N47" t="s">
+        <v>36</v>
+      </c>
+      <c r="O47" t="s">
+        <v>37</v>
+      </c>
+      <c r="P47" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>117</v>
+      </c>
+      <c r="R47" t="s">
+        <v>290</v>
+      </c>
+      <c r="S47" t="s">
+        <v>291</v>
+      </c>
+      <c r="T47" t="s">
+        <v>315</v>
+      </c>
+      <c r="U47" t="s">
+        <v>316</v>
+      </c>
+      <c r="V47" t="s">
+        <v>231</v>
+      </c>
+      <c r="X47" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>113</v>
+      </c>
+      <c r="C48" t="s">
+        <v>317</v>
+      </c>
+      <c r="D48" t="s">
+        <v>125</v>
+      </c>
+      <c r="E48" t="s">
+        <v>261</v>
+      </c>
+      <c r="F48" t="s">
+        <v>242</v>
+      </c>
+      <c r="G48" t="s">
+        <v>238</v>
+      </c>
+      <c r="H48" t="s">
+        <v>244</v>
+      </c>
+      <c r="I48" t="s">
+        <v>240</v>
+      </c>
+      <c r="J48" t="s">
+        <v>222</v>
+      </c>
+      <c r="K48" t="s">
+        <v>155</v>
+      </c>
+      <c r="L48" t="s">
+        <v>35</v>
+      </c>
+      <c r="M48" t="s">
+        <v>35</v>
+      </c>
+      <c r="N48" t="s">
+        <v>36</v>
+      </c>
+      <c r="O48" t="s">
+        <v>37</v>
+      </c>
+      <c r="P48" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q48" t="s">
+        <v>117</v>
+      </c>
+      <c r="R48" t="s">
+        <v>290</v>
+      </c>
+      <c r="S48" t="s">
+        <v>285</v>
+      </c>
+      <c r="T48" t="s">
+        <v>318</v>
+      </c>
+      <c r="U48" t="s">
+        <v>229</v>
+      </c>
+      <c r="V48" t="s">
+        <v>231</v>
+      </c>
+      <c r="X48" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>113</v>
+      </c>
+      <c r="C49" t="s">
+        <v>319</v>
+      </c>
+      <c r="D49" t="s">
+        <v>153</v>
+      </c>
+      <c r="E49" t="s">
+        <v>154</v>
+      </c>
+      <c r="F49" t="s">
+        <v>137</v>
+      </c>
+      <c r="G49" t="s">
+        <v>238</v>
+      </c>
+      <c r="H49" t="s">
+        <v>244</v>
+      </c>
+      <c r="I49" t="s">
+        <v>240</v>
+      </c>
+      <c r="J49" t="s">
+        <v>222</v>
+      </c>
+      <c r="K49" t="s">
+        <v>155</v>
+      </c>
+      <c r="L49" t="s">
+        <v>35</v>
+      </c>
+      <c r="M49" t="s">
+        <v>35</v>
+      </c>
+      <c r="N49" t="s">
+        <v>36</v>
+      </c>
+      <c r="O49" t="s">
+        <v>37</v>
+      </c>
+      <c r="P49" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>117</v>
+      </c>
+      <c r="R49" t="s">
+        <v>290</v>
+      </c>
+      <c r="S49" t="s">
+        <v>291</v>
+      </c>
+      <c r="T49" t="s">
+        <v>292</v>
+      </c>
+      <c r="U49" t="s">
+        <v>293</v>
+      </c>
+      <c r="V49" t="s">
+        <v>273</v>
+      </c>
+      <c r="W49" t="s">
+        <v>320</v>
+      </c>
+      <c r="X49" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>113</v>
+      </c>
+      <c r="C50" t="s">
+        <v>321</v>
+      </c>
+      <c r="D50" t="s">
+        <v>153</v>
+      </c>
+      <c r="E50" t="s">
+        <v>154</v>
+      </c>
+      <c r="F50" t="s">
+        <v>137</v>
+      </c>
+      <c r="G50" t="s">
+        <v>238</v>
+      </c>
+      <c r="H50" t="s">
+        <v>244</v>
+      </c>
+      <c r="I50" t="s">
+        <v>240</v>
+      </c>
+      <c r="J50" t="s">
+        <v>222</v>
+      </c>
+      <c r="K50" t="s">
+        <v>155</v>
+      </c>
+      <c r="L50" t="s">
+        <v>35</v>
+      </c>
+      <c r="M50" t="s">
+        <v>35</v>
+      </c>
+      <c r="N50" t="s">
+        <v>36</v>
+      </c>
+      <c r="O50" t="s">
+        <v>37</v>
+      </c>
+      <c r="P50" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>117</v>
+      </c>
+      <c r="R50" t="s">
+        <v>290</v>
+      </c>
+      <c r="S50" t="s">
+        <v>291</v>
+      </c>
+      <c r="T50" t="s">
+        <v>292</v>
+      </c>
+      <c r="U50" t="s">
+        <v>293</v>
+      </c>
+      <c r="V50" t="s">
+        <v>273</v>
+      </c>
+      <c r="W50" t="s">
+        <v>320</v>
+      </c>
+      <c r="X50" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>113</v>
+      </c>
+      <c r="C51" t="s">
+        <v>322</v>
+      </c>
+      <c r="D51" t="s">
+        <v>296</v>
+      </c>
+      <c r="E51" t="s">
+        <v>297</v>
+      </c>
+      <c r="F51" t="s">
+        <v>137</v>
+      </c>
+      <c r="G51" t="s">
+        <v>238</v>
+      </c>
+      <c r="H51" t="s">
+        <v>265</v>
+      </c>
+      <c r="I51" t="s">
+        <v>240</v>
+      </c>
+      <c r="J51" t="s">
+        <v>222</v>
+      </c>
+      <c r="K51" t="s">
+        <v>155</v>
+      </c>
+      <c r="L51" t="s">
+        <v>35</v>
+      </c>
+      <c r="M51" t="s">
+        <v>35</v>
+      </c>
+      <c r="N51" t="s">
+        <v>36</v>
+      </c>
+      <c r="O51" t="s">
+        <v>37</v>
+      </c>
+      <c r="P51" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q51" t="s">
+        <v>38</v>
+      </c>
+      <c r="R51" t="s">
+        <v>299</v>
+      </c>
+      <c r="S51" t="s">
+        <v>268</v>
+      </c>
+      <c r="T51" t="s">
+        <v>270</v>
+      </c>
+      <c r="U51" t="s">
+        <v>286</v>
+      </c>
+      <c r="V51" t="s">
+        <v>273</v>
+      </c>
+      <c r="X51" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>113</v>
+      </c>
+      <c r="C52" t="s">
+        <v>323</v>
+      </c>
+      <c r="D52" t="s">
+        <v>324</v>
+      </c>
+      <c r="E52" t="s">
+        <v>261</v>
+      </c>
+      <c r="F52" t="s">
+        <v>263</v>
+      </c>
+      <c r="G52" t="s">
+        <v>238</v>
+      </c>
+      <c r="H52" t="s">
+        <v>244</v>
+      </c>
+      <c r="I52" t="s">
+        <v>240</v>
+      </c>
+      <c r="J52" t="s">
+        <v>222</v>
+      </c>
+      <c r="K52" t="s">
+        <v>155</v>
+      </c>
+      <c r="L52" t="s">
+        <v>35</v>
+      </c>
+      <c r="M52" t="s">
+        <v>35</v>
+      </c>
+      <c r="N52" t="s">
+        <v>36</v>
+      </c>
+      <c r="O52" t="s">
+        <v>37</v>
+      </c>
+      <c r="P52" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q52" t="s">
+        <v>38</v>
+      </c>
+      <c r="R52" t="s">
+        <v>305</v>
+      </c>
+      <c r="S52" t="s">
+        <v>306</v>
+      </c>
+      <c r="T52" t="s">
+        <v>255</v>
+      </c>
+      <c r="U52" t="s">
+        <v>307</v>
+      </c>
+      <c r="V52" t="s">
+        <v>273</v>
+      </c>
+      <c r="X52" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>113</v>
+      </c>
+      <c r="C53" t="s">
+        <v>325</v>
+      </c>
+      <c r="D53" t="s">
+        <v>303</v>
+      </c>
+      <c r="E53" t="s">
+        <v>304</v>
+      </c>
+      <c r="F53" t="s">
+        <v>137</v>
+      </c>
+      <c r="G53" t="s">
+        <v>238</v>
+      </c>
+      <c r="H53" t="s">
+        <v>244</v>
+      </c>
+      <c r="I53" t="s">
+        <v>240</v>
+      </c>
+      <c r="J53" t="s">
+        <v>222</v>
+      </c>
+      <c r="K53" t="s">
+        <v>155</v>
+      </c>
+      <c r="L53" t="s">
+        <v>35</v>
+      </c>
+      <c r="M53" t="s">
+        <v>35</v>
+      </c>
+      <c r="N53" t="s">
+        <v>36</v>
+      </c>
+      <c r="O53" t="s">
+        <v>37</v>
+      </c>
+      <c r="P53" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>38</v>
+      </c>
+      <c r="R53" t="s">
+        <v>305</v>
+      </c>
+      <c r="S53" t="s">
+        <v>306</v>
+      </c>
+      <c r="T53" t="s">
+        <v>255</v>
+      </c>
+      <c r="U53" t="s">
+        <v>307</v>
+      </c>
+      <c r="V53" t="s">
+        <v>273</v>
+      </c>
+      <c r="W53" t="s">
+        <v>326</v>
+      </c>
+      <c r="X53" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>113</v>
+      </c>
+      <c r="C54" t="s">
+        <v>327</v>
+      </c>
+      <c r="D54" t="s">
+        <v>328</v>
+      </c>
+      <c r="E54" t="s">
+        <v>329</v>
+      </c>
+      <c r="F54" t="s">
+        <v>137</v>
+      </c>
+      <c r="G54" t="s">
+        <v>238</v>
+      </c>
+      <c r="H54" t="s">
+        <v>244</v>
+      </c>
+      <c r="I54" t="s">
+        <v>240</v>
+      </c>
+      <c r="J54" t="s">
+        <v>222</v>
+      </c>
+      <c r="K54" t="s">
+        <v>155</v>
+      </c>
+      <c r="L54" t="s">
+        <v>35</v>
+      </c>
+      <c r="M54" t="s">
+        <v>35</v>
+      </c>
+      <c r="N54" t="s">
+        <v>36</v>
+      </c>
+      <c r="O54" t="s">
+        <v>37</v>
+      </c>
+      <c r="P54" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>117</v>
+      </c>
+      <c r="R54" t="s">
+        <v>290</v>
+      </c>
+      <c r="S54" t="s">
+        <v>291</v>
+      </c>
+      <c r="T54" t="s">
+        <v>292</v>
+      </c>
+      <c r="U54" t="s">
+        <v>293</v>
+      </c>
+      <c r="V54" t="s">
+        <v>294</v>
+      </c>
+      <c r="X54" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" t="s">
+        <v>330</v>
+      </c>
+      <c r="D55" t="s">
+        <v>328</v>
+      </c>
+      <c r="E55" t="s">
+        <v>329</v>
+      </c>
+      <c r="F55" t="s">
+        <v>331</v>
+      </c>
+      <c r="G55" t="s">
+        <v>238</v>
+      </c>
+      <c r="H55" t="s">
+        <v>244</v>
+      </c>
+      <c r="I55" t="s">
+        <v>240</v>
+      </c>
+      <c r="J55" t="s">
+        <v>222</v>
+      </c>
+      <c r="K55" t="s">
+        <v>155</v>
+      </c>
+      <c r="L55" t="s">
+        <v>35</v>
+      </c>
+      <c r="M55" t="s">
+        <v>35</v>
+      </c>
+      <c r="N55" t="s">
+        <v>36</v>
+      </c>
+      <c r="O55" t="s">
+        <v>37</v>
+      </c>
+      <c r="P55" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>117</v>
+      </c>
+      <c r="R55" t="s">
+        <v>290</v>
+      </c>
+      <c r="S55" t="s">
+        <v>291</v>
+      </c>
+      <c r="T55" t="s">
+        <v>292</v>
+      </c>
+      <c r="U55" t="s">
+        <v>293</v>
+      </c>
+      <c r="V55" t="s">
+        <v>294</v>
+      </c>
+      <c r="X55" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>113</v>
+      </c>
+      <c r="C56" t="s">
+        <v>332</v>
+      </c>
+      <c r="D56" t="s">
+        <v>333</v>
+      </c>
+      <c r="E56" t="s">
+        <v>334</v>
+      </c>
+      <c r="F56" t="s">
+        <v>137</v>
+      </c>
+      <c r="G56" t="s">
+        <v>238</v>
+      </c>
+      <c r="H56" t="s">
+        <v>265</v>
+      </c>
+      <c r="I56" t="s">
+        <v>240</v>
+      </c>
+      <c r="J56" t="s">
+        <v>222</v>
+      </c>
+      <c r="K56" t="s">
+        <v>155</v>
+      </c>
+      <c r="L56" t="s">
+        <v>35</v>
+      </c>
+      <c r="M56" t="s">
+        <v>35</v>
+      </c>
+      <c r="N56" t="s">
+        <v>36</v>
+      </c>
+      <c r="O56" t="s">
+        <v>37</v>
+      </c>
+      <c r="P56" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>38</v>
+      </c>
+      <c r="R56" t="s">
+        <v>335</v>
+      </c>
+      <c r="S56" t="s">
+        <v>269</v>
+      </c>
+      <c r="T56" t="s">
+        <v>271</v>
+      </c>
+      <c r="U56" t="s">
+        <v>229</v>
+      </c>
+      <c r="V56" t="s">
+        <v>231</v>
+      </c>
+      <c r="X56" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>113</v>
+      </c>
+      <c r="C57" t="s">
+        <v>336</v>
+      </c>
+      <c r="D57" t="s">
+        <v>337</v>
+      </c>
+      <c r="E57" t="s">
+        <v>304</v>
+      </c>
+      <c r="F57" t="s">
+        <v>137</v>
+      </c>
+      <c r="G57" t="s">
+        <v>238</v>
+      </c>
+      <c r="H57" t="s">
+        <v>244</v>
+      </c>
+      <c r="I57" t="s">
+        <v>240</v>
+      </c>
+      <c r="J57" t="s">
+        <v>222</v>
+      </c>
+      <c r="K57" t="s">
+        <v>155</v>
+      </c>
+      <c r="L57" t="s">
+        <v>35</v>
+      </c>
+      <c r="M57" t="s">
+        <v>35</v>
+      </c>
+      <c r="N57" t="s">
+        <v>36</v>
+      </c>
+      <c r="O57" t="s">
+        <v>37</v>
+      </c>
+      <c r="P57" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>117</v>
+      </c>
+      <c r="R57" t="s">
+        <v>338</v>
+      </c>
+      <c r="S57" t="s">
+        <v>339</v>
+      </c>
+      <c r="T57" t="s">
+        <v>340</v>
+      </c>
+      <c r="U57" t="s">
+        <v>307</v>
+      </c>
+      <c r="V57" t="s">
+        <v>294</v>
+      </c>
+      <c r="W57" t="s">
+        <v>341</v>
+      </c>
+      <c r="X57" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>113</v>
+      </c>
+      <c r="C58" t="s">
+        <v>342</v>
+      </c>
+      <c r="D58" t="s">
+        <v>343</v>
+      </c>
+      <c r="E58" t="s">
+        <v>344</v>
+      </c>
+      <c r="F58" t="s">
+        <v>263</v>
+      </c>
+      <c r="G58" t="s">
+        <v>238</v>
+      </c>
+      <c r="H58" t="s">
+        <v>265</v>
+      </c>
+      <c r="I58" t="s">
+        <v>240</v>
+      </c>
+      <c r="J58" t="s">
+        <v>222</v>
+      </c>
+      <c r="K58" t="s">
+        <v>155</v>
+      </c>
+      <c r="L58" t="s">
+        <v>35</v>
+      </c>
+      <c r="M58" t="s">
+        <v>35</v>
+      </c>
+      <c r="N58" t="s">
+        <v>36</v>
+      </c>
+      <c r="O58" t="s">
+        <v>37</v>
+      </c>
+      <c r="P58" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>38</v>
+      </c>
+      <c r="R58" t="s">
+        <v>345</v>
+      </c>
+      <c r="S58" t="s">
+        <v>269</v>
+      </c>
+      <c r="T58" t="s">
+        <v>271</v>
+      </c>
+      <c r="U58" t="s">
+        <v>229</v>
+      </c>
+      <c r="V58" t="s">
+        <v>231</v>
+      </c>
+      <c r="X58" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>113</v>
+      </c>
+      <c r="C59" t="s">
+        <v>346</v>
+      </c>
+      <c r="D59" t="s">
+        <v>347</v>
+      </c>
+      <c r="E59" t="s">
+        <v>348</v>
+      </c>
+      <c r="F59" t="s">
+        <v>137</v>
+      </c>
+      <c r="G59" t="s">
+        <v>238</v>
+      </c>
+      <c r="H59" t="s">
+        <v>239</v>
+      </c>
+      <c r="I59" t="s">
+        <v>240</v>
+      </c>
+      <c r="J59" t="s">
+        <v>222</v>
+      </c>
+      <c r="K59" t="s">
+        <v>155</v>
+      </c>
+      <c r="L59" t="s">
+        <v>35</v>
+      </c>
+      <c r="M59" t="s">
+        <v>35</v>
+      </c>
+      <c r="N59" t="s">
+        <v>36</v>
+      </c>
+      <c r="O59" t="s">
+        <v>37</v>
+      </c>
+      <c r="P59" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>117</v>
+      </c>
+      <c r="R59" t="s">
+        <v>349</v>
+      </c>
+      <c r="S59" t="s">
+        <v>285</v>
+      </c>
+      <c r="T59" t="s">
+        <v>318</v>
+      </c>
+      <c r="U59" t="s">
+        <v>316</v>
+      </c>
+      <c r="V59" t="s">
+        <v>231</v>
+      </c>
+      <c r="X59" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>113</v>
+      </c>
+      <c r="C60" t="s">
+        <v>350</v>
+      </c>
+      <c r="D60" t="s">
+        <v>351</v>
+      </c>
+      <c r="E60" t="s">
+        <v>352</v>
+      </c>
+      <c r="F60" t="s">
+        <v>137</v>
+      </c>
+      <c r="G60" t="s">
+        <v>238</v>
+      </c>
+      <c r="H60" t="s">
+        <v>244</v>
+      </c>
+      <c r="I60" t="s">
+        <v>240</v>
+      </c>
+      <c r="J60" t="s">
+        <v>222</v>
+      </c>
+      <c r="K60" t="s">
+        <v>155</v>
+      </c>
+      <c r="L60" t="s">
+        <v>35</v>
+      </c>
+      <c r="M60" t="s">
+        <v>35</v>
+      </c>
+      <c r="N60" t="s">
+        <v>36</v>
+      </c>
+      <c r="O60" t="s">
+        <v>37</v>
+      </c>
+      <c r="P60" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>117</v>
+      </c>
+      <c r="R60" t="s">
+        <v>349</v>
+      </c>
+      <c r="S60" t="s">
+        <v>353</v>
+      </c>
+      <c r="T60" t="s">
+        <v>340</v>
+      </c>
+      <c r="U60" t="s">
+        <v>307</v>
+      </c>
+      <c r="V60" t="s">
+        <v>273</v>
+      </c>
+      <c r="W60" t="s">
+        <v>354</v>
+      </c>
+      <c r="X60" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>113</v>
+      </c>
+      <c r="C61" t="s">
+        <v>355</v>
+      </c>
+      <c r="D61" t="s">
+        <v>356</v>
+      </c>
+      <c r="E61" t="s">
+        <v>329</v>
+      </c>
+      <c r="F61" t="s">
+        <v>137</v>
+      </c>
+      <c r="G61" t="s">
+        <v>238</v>
+      </c>
+      <c r="H61" t="s">
+        <v>239</v>
+      </c>
+      <c r="I61" t="s">
+        <v>240</v>
+      </c>
+      <c r="J61" t="s">
+        <v>222</v>
+      </c>
+      <c r="K61" t="s">
+        <v>155</v>
+      </c>
+      <c r="L61" t="s">
+        <v>35</v>
+      </c>
+      <c r="M61" t="s">
+        <v>35</v>
+      </c>
+      <c r="N61" t="s">
+        <v>36</v>
+      </c>
+      <c r="O61" t="s">
+        <v>37</v>
+      </c>
+      <c r="P61" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q61" t="s">
+        <v>117</v>
+      </c>
+      <c r="R61" t="s">
+        <v>357</v>
+      </c>
+      <c r="S61" t="s">
+        <v>285</v>
+      </c>
+      <c r="T61" t="s">
+        <v>318</v>
+      </c>
+      <c r="U61" t="s">
+        <v>229</v>
+      </c>
+      <c r="V61" t="s">
+        <v>231</v>
+      </c>
+      <c r="X61" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>113</v>
+      </c>
+      <c r="C62" t="s">
+        <v>358</v>
+      </c>
+      <c r="D62" t="s">
+        <v>359</v>
+      </c>
+      <c r="E62" t="s">
+        <v>311</v>
+      </c>
+      <c r="F62" t="s">
+        <v>137</v>
+      </c>
+      <c r="G62" t="s">
+        <v>238</v>
+      </c>
+      <c r="H62" t="s">
+        <v>244</v>
+      </c>
+      <c r="I62" t="s">
+        <v>240</v>
+      </c>
+      <c r="J62" t="s">
+        <v>222</v>
+      </c>
+      <c r="K62" t="s">
+        <v>155</v>
+      </c>
+      <c r="L62" t="s">
+        <v>35</v>
+      </c>
+      <c r="M62" t="s">
+        <v>35</v>
+      </c>
+      <c r="N62" t="s">
+        <v>36</v>
+      </c>
+      <c r="O62" t="s">
+        <v>37</v>
+      </c>
+      <c r="P62" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>117</v>
+      </c>
+      <c r="R62" t="s">
+        <v>360</v>
+      </c>
+      <c r="S62" t="s">
+        <v>361</v>
+      </c>
+      <c r="T62" t="s">
+        <v>318</v>
+      </c>
+      <c r="U62" t="s">
+        <v>229</v>
+      </c>
+      <c r="V62" t="s">
+        <v>273</v>
+      </c>
+      <c r="X62" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>113</v>
+      </c>
+      <c r="C63" t="s">
+        <v>362</v>
+      </c>
+      <c r="D63" t="s">
+        <v>363</v>
+      </c>
+      <c r="E63" t="s">
+        <v>304</v>
+      </c>
+      <c r="F63" t="s">
+        <v>137</v>
+      </c>
+      <c r="G63" t="s">
+        <v>238</v>
+      </c>
+      <c r="H63" t="s">
+        <v>244</v>
+      </c>
+      <c r="I63" t="s">
+        <v>240</v>
+      </c>
+      <c r="J63" t="s">
+        <v>222</v>
+      </c>
+      <c r="K63" t="s">
+        <v>155</v>
+      </c>
+      <c r="L63" t="s">
+        <v>35</v>
+      </c>
+      <c r="M63" t="s">
+        <v>35</v>
+      </c>
+      <c r="N63" t="s">
+        <v>36</v>
+      </c>
+      <c r="O63" t="s">
+        <v>37</v>
+      </c>
+      <c r="P63" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>117</v>
+      </c>
+      <c r="R63" t="s">
+        <v>338</v>
+      </c>
+      <c r="S63" t="s">
+        <v>339</v>
+      </c>
+      <c r="T63" t="s">
+        <v>340</v>
+      </c>
+      <c r="U63" t="s">
+        <v>307</v>
+      </c>
+      <c r="V63" t="s">
+        <v>294</v>
+      </c>
+      <c r="X63" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>113</v>
+      </c>
+      <c r="C64" t="s">
+        <v>364</v>
+      </c>
+      <c r="D64" t="s">
+        <v>365</v>
+      </c>
+      <c r="E64" t="s">
+        <v>329</v>
+      </c>
+      <c r="F64" t="s">
+        <v>263</v>
+      </c>
+      <c r="G64" t="s">
+        <v>238</v>
+      </c>
+      <c r="H64" t="s">
+        <v>265</v>
+      </c>
+      <c r="I64" t="s">
+        <v>240</v>
+      </c>
+      <c r="J64" t="s">
+        <v>222</v>
+      </c>
+      <c r="K64" t="s">
+        <v>155</v>
+      </c>
+      <c r="L64" t="s">
+        <v>35</v>
+      </c>
+      <c r="M64" t="s">
+        <v>35</v>
+      </c>
+      <c r="N64" t="s">
+        <v>36</v>
+      </c>
+      <c r="O64" t="s">
+        <v>37</v>
+      </c>
+      <c r="P64" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>38</v>
+      </c>
+      <c r="R64" t="s">
+        <v>335</v>
+      </c>
+      <c r="S64" t="s">
+        <v>268</v>
+      </c>
+      <c r="T64" t="s">
+        <v>270</v>
+      </c>
+      <c r="U64" t="s">
+        <v>272</v>
+      </c>
+      <c r="V64" t="s">
+        <v>366</v>
+      </c>
+      <c r="W64" t="s">
+        <v>367</v>
+      </c>
+      <c r="X64" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="65" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>113</v>
+      </c>
+      <c r="C65" t="s">
+        <v>368</v>
+      </c>
+      <c r="D65" t="s">
+        <v>369</v>
+      </c>
+      <c r="E65" t="s">
+        <v>370</v>
+      </c>
+      <c r="F65" t="s">
+        <v>137</v>
+      </c>
+      <c r="G65" t="s">
+        <v>238</v>
+      </c>
+      <c r="H65" t="s">
+        <v>371</v>
+      </c>
+      <c r="I65" t="s">
+        <v>240</v>
+      </c>
+      <c r="J65" t="s">
+        <v>222</v>
+      </c>
+      <c r="K65" t="s">
+        <v>155</v>
+      </c>
+      <c r="L65" t="s">
+        <v>35</v>
+      </c>
+      <c r="M65" t="s">
+        <v>35</v>
+      </c>
+      <c r="N65" t="s">
+        <v>36</v>
+      </c>
+      <c r="O65" t="s">
+        <v>37</v>
+      </c>
+      <c r="P65" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>38</v>
+      </c>
+      <c r="R65" t="s">
+        <v>345</v>
+      </c>
+      <c r="S65" t="s">
+        <v>306</v>
+      </c>
+      <c r="T65" t="s">
+        <v>255</v>
+      </c>
+      <c r="U65" t="s">
+        <v>307</v>
+      </c>
+      <c r="V65" t="s">
+        <v>294</v>
+      </c>
+      <c r="W65" t="s">
+        <v>372</v>
+      </c>
+      <c r="X65" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="66" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>113</v>
+      </c>
+      <c r="C66" t="s">
+        <v>373</v>
+      </c>
+      <c r="D66" t="s">
+        <v>356</v>
+      </c>
+      <c r="E66" t="s">
+        <v>329</v>
+      </c>
+      <c r="F66" t="s">
+        <v>137</v>
+      </c>
+      <c r="G66" t="s">
+        <v>238</v>
+      </c>
+      <c r="H66" t="s">
+        <v>243</v>
+      </c>
+      <c r="I66" t="s">
+        <v>240</v>
+      </c>
+      <c r="J66" t="s">
+        <v>222</v>
+      </c>
+      <c r="K66" t="s">
+        <v>155</v>
+      </c>
+      <c r="L66" t="s">
+        <v>35</v>
+      </c>
+      <c r="M66" t="s">
+        <v>35</v>
+      </c>
+      <c r="N66" t="s">
+        <v>36</v>
+      </c>
+      <c r="O66" t="s">
+        <v>37</v>
+      </c>
+      <c r="P66" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>117</v>
+      </c>
+      <c r="R66" t="s">
+        <v>357</v>
+      </c>
+      <c r="S66" t="s">
+        <v>353</v>
+      </c>
+      <c r="T66" t="s">
+        <v>340</v>
+      </c>
+      <c r="U66" t="s">
+        <v>307</v>
+      </c>
+      <c r="V66" t="s">
+        <v>273</v>
+      </c>
+      <c r="X66" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="67" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>113</v>
+      </c>
+      <c r="C67" t="s">
+        <v>374</v>
+      </c>
+      <c r="D67" t="s">
+        <v>375</v>
+      </c>
+      <c r="E67" t="s">
+        <v>329</v>
+      </c>
+      <c r="F67" t="s">
+        <v>263</v>
+      </c>
+      <c r="G67" t="s">
+        <v>238</v>
+      </c>
+      <c r="H67" t="s">
+        <v>265</v>
+      </c>
+      <c r="I67" t="s">
+        <v>240</v>
+      </c>
+      <c r="J67" t="s">
+        <v>222</v>
+      </c>
+      <c r="K67" t="s">
+        <v>155</v>
+      </c>
+      <c r="L67" t="s">
+        <v>35</v>
+      </c>
+      <c r="M67" t="s">
+        <v>35</v>
+      </c>
+      <c r="N67" t="s">
+        <v>36</v>
+      </c>
+      <c r="O67" t="s">
+        <v>37</v>
+      </c>
+      <c r="P67" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>38</v>
+      </c>
+      <c r="R67" t="s">
+        <v>335</v>
+      </c>
+      <c r="S67" t="s">
+        <v>268</v>
+      </c>
+      <c r="T67" t="s">
+        <v>270</v>
+      </c>
+      <c r="U67" t="s">
+        <v>272</v>
+      </c>
+      <c r="V67" t="s">
+        <v>273</v>
+      </c>
+      <c r="W67" t="s">
+        <v>376</v>
+      </c>
+      <c r="X67" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="68" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>113</v>
+      </c>
+      <c r="C68" t="s">
+        <v>377</v>
+      </c>
+      <c r="D68" t="s">
+        <v>378</v>
+      </c>
+      <c r="E68" t="s">
+        <v>344</v>
+      </c>
+      <c r="F68" t="s">
+        <v>263</v>
+      </c>
+      <c r="G68" t="s">
+        <v>238</v>
+      </c>
+      <c r="H68" t="s">
+        <v>244</v>
+      </c>
+      <c r="I68" t="s">
+        <v>240</v>
+      </c>
+      <c r="J68" t="s">
+        <v>222</v>
+      </c>
+      <c r="K68" t="s">
+        <v>155</v>
+      </c>
+      <c r="L68" t="s">
+        <v>35</v>
+      </c>
+      <c r="M68" t="s">
+        <v>35</v>
+      </c>
+      <c r="N68" t="s">
+        <v>36</v>
+      </c>
+      <c r="O68" t="s">
+        <v>37</v>
+      </c>
+      <c r="P68" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>38</v>
+      </c>
+      <c r="R68" t="s">
+        <v>345</v>
+      </c>
+      <c r="S68" t="s">
+        <v>269</v>
+      </c>
+      <c r="T68" t="s">
+        <v>271</v>
+      </c>
+      <c r="U68" t="s">
+        <v>229</v>
+      </c>
+      <c r="V68" t="s">
+        <v>231</v>
+      </c>
+      <c r="X68" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="69" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>113</v>
+      </c>
+      <c r="C69" t="s">
+        <v>419</v>
+      </c>
+      <c r="D69" t="s">
+        <v>408</v>
+      </c>
+      <c r="E69" t="s">
+        <v>398</v>
+      </c>
+      <c r="F69" t="s">
+        <v>263</v>
+      </c>
+      <c r="G69" t="s">
+        <v>238</v>
+      </c>
+      <c r="H69" t="s">
+        <v>265</v>
+      </c>
+      <c r="I69" t="s">
+        <v>240</v>
+      </c>
+      <c r="J69" t="s">
+        <v>222</v>
+      </c>
+      <c r="K69" t="s">
+        <v>155</v>
+      </c>
+      <c r="L69" t="s">
+        <v>35</v>
+      </c>
+      <c r="M69" t="s">
+        <v>35</v>
+      </c>
+      <c r="N69" t="s">
+        <v>36</v>
+      </c>
+      <c r="O69" t="s">
+        <v>37</v>
+      </c>
+      <c r="P69" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>38</v>
+      </c>
+      <c r="R69" t="s">
+        <v>393</v>
+      </c>
+      <c r="S69" t="s">
+        <v>268</v>
+      </c>
+      <c r="T69" t="s">
+        <v>270</v>
+      </c>
+      <c r="U69" t="s">
+        <v>384</v>
+      </c>
+      <c r="V69" t="s">
+        <v>231</v>
+      </c>
+      <c r="W69" t="s">
+        <v>380</v>
+      </c>
+      <c r="X69" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="70" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>113</v>
+      </c>
+      <c r="C70" t="s">
+        <v>418</v>
+      </c>
+      <c r="D70" t="s">
+        <v>407</v>
+      </c>
+      <c r="E70" t="s">
+        <v>304</v>
+      </c>
+      <c r="F70" t="s">
+        <v>137</v>
+      </c>
+      <c r="G70" t="s">
+        <v>238</v>
+      </c>
+      <c r="H70" t="s">
+        <v>265</v>
+      </c>
+      <c r="I70" t="s">
+        <v>240</v>
+      </c>
+      <c r="J70" t="s">
+        <v>222</v>
+      </c>
+      <c r="K70" t="s">
+        <v>155</v>
+      </c>
+      <c r="L70" t="s">
+        <v>35</v>
+      </c>
+      <c r="M70" t="s">
+        <v>35</v>
+      </c>
+      <c r="N70" t="s">
+        <v>36</v>
+      </c>
+      <c r="O70" t="s">
+        <v>37</v>
+      </c>
+      <c r="P70" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q70" t="s">
+        <v>38</v>
+      </c>
+      <c r="R70" t="s">
+        <v>393</v>
+      </c>
+      <c r="S70" t="s">
+        <v>268</v>
+      </c>
+      <c r="T70" t="s">
+        <v>270</v>
+      </c>
+      <c r="U70" t="s">
+        <v>384</v>
+      </c>
+      <c r="V70" t="s">
+        <v>273</v>
+      </c>
+      <c r="W70" t="s">
+        <v>380</v>
+      </c>
+      <c r="X70" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="71" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>113</v>
+      </c>
+      <c r="C71" t="s">
+        <v>417</v>
+      </c>
+      <c r="D71" t="s">
+        <v>406</v>
+      </c>
+      <c r="E71" t="s">
+        <v>329</v>
+      </c>
+      <c r="F71" t="s">
+        <v>263</v>
+      </c>
+      <c r="G71" t="s">
+        <v>238</v>
+      </c>
+      <c r="H71" t="s">
+        <v>244</v>
+      </c>
+      <c r="I71" t="s">
+        <v>240</v>
+      </c>
+      <c r="J71" t="s">
+        <v>222</v>
+      </c>
+      <c r="K71" t="s">
+        <v>155</v>
+      </c>
+      <c r="L71" t="s">
+        <v>35</v>
+      </c>
+      <c r="M71" t="s">
+        <v>35</v>
+      </c>
+      <c r="N71" t="s">
+        <v>36</v>
+      </c>
+      <c r="O71" t="s">
+        <v>37</v>
+      </c>
+      <c r="P71" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>38</v>
+      </c>
+      <c r="R71" t="s">
+        <v>393</v>
+      </c>
+      <c r="S71" t="s">
+        <v>268</v>
+      </c>
+      <c r="T71" t="s">
+        <v>270</v>
+      </c>
+      <c r="U71" t="s">
+        <v>384</v>
+      </c>
+      <c r="V71" t="s">
+        <v>273</v>
+      </c>
+      <c r="W71" t="s">
+        <v>380</v>
+      </c>
+      <c r="X71" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="72" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>113</v>
+      </c>
+      <c r="C72" t="s">
+        <v>413</v>
+      </c>
+      <c r="D72" t="s">
+        <v>403</v>
+      </c>
+      <c r="E72" t="s">
+        <v>344</v>
+      </c>
+      <c r="F72" t="s">
+        <v>137</v>
+      </c>
+      <c r="G72" t="s">
+        <v>238</v>
+      </c>
+      <c r="H72" t="s">
+        <v>244</v>
+      </c>
+      <c r="I72" t="s">
+        <v>240</v>
+      </c>
+      <c r="J72" t="s">
+        <v>222</v>
+      </c>
+      <c r="K72" t="s">
+        <v>155</v>
+      </c>
+      <c r="L72" t="s">
+        <v>35</v>
+      </c>
+      <c r="M72" t="s">
+        <v>35</v>
+      </c>
+      <c r="N72" t="s">
+        <v>36</v>
+      </c>
+      <c r="O72" t="s">
+        <v>37</v>
+      </c>
+      <c r="P72" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>38</v>
+      </c>
+      <c r="R72" t="s">
+        <v>393</v>
+      </c>
+      <c r="S72" t="s">
+        <v>269</v>
+      </c>
+      <c r="T72" t="s">
+        <v>387</v>
+      </c>
+      <c r="U72" t="s">
+        <v>381</v>
+      </c>
+      <c r="V72" t="s">
+        <v>231</v>
+      </c>
+      <c r="X72" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="73" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>113</v>
+      </c>
+      <c r="C73" t="s">
+        <v>416</v>
+      </c>
+      <c r="D73" t="s">
+        <v>400</v>
+      </c>
+      <c r="E73" t="s">
+        <v>154</v>
+      </c>
+      <c r="F73" t="s">
+        <v>263</v>
+      </c>
+      <c r="G73" t="s">
+        <v>238</v>
+      </c>
+      <c r="H73" t="s">
+        <v>265</v>
+      </c>
+      <c r="I73" t="s">
+        <v>240</v>
+      </c>
+      <c r="J73" t="s">
+        <v>222</v>
+      </c>
+      <c r="K73" t="s">
+        <v>155</v>
+      </c>
+      <c r="L73" t="s">
+        <v>35</v>
+      </c>
+      <c r="M73" t="s">
+        <v>35</v>
+      </c>
+      <c r="N73" t="s">
+        <v>36</v>
+      </c>
+      <c r="O73" t="s">
+        <v>37</v>
+      </c>
+      <c r="P73" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>38</v>
+      </c>
+      <c r="R73" t="s">
+        <v>394</v>
+      </c>
+      <c r="S73" t="s">
+        <v>389</v>
+      </c>
+      <c r="T73" t="s">
+        <v>387</v>
+      </c>
+      <c r="U73" t="s">
+        <v>383</v>
+      </c>
+      <c r="V73" t="s">
+        <v>231</v>
+      </c>
+      <c r="W73" t="s">
+        <v>379</v>
+      </c>
+      <c r="X73" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="74" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>113</v>
+      </c>
+      <c r="C74" t="s">
+        <v>415</v>
+      </c>
+      <c r="D74" t="s">
+        <v>405</v>
+      </c>
+      <c r="E74" t="s">
+        <v>311</v>
+      </c>
+      <c r="F74" t="s">
+        <v>137</v>
+      </c>
+      <c r="G74" t="s">
+        <v>238</v>
+      </c>
+      <c r="H74" t="s">
+        <v>244</v>
+      </c>
+      <c r="I74" t="s">
+        <v>240</v>
+      </c>
+      <c r="J74" t="s">
+        <v>222</v>
+      </c>
+      <c r="K74" t="s">
+        <v>155</v>
+      </c>
+      <c r="L74" t="s">
+        <v>35</v>
+      </c>
+      <c r="M74" t="s">
+        <v>35</v>
+      </c>
+      <c r="N74" t="s">
+        <v>36</v>
+      </c>
+      <c r="O74" t="s">
+        <v>37</v>
+      </c>
+      <c r="P74" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q74" t="s">
+        <v>38</v>
+      </c>
+      <c r="R74" t="s">
+        <v>390</v>
+      </c>
+      <c r="S74" t="s">
+        <v>269</v>
+      </c>
+      <c r="T74" t="s">
+        <v>271</v>
+      </c>
+      <c r="U74" t="s">
+        <v>381</v>
+      </c>
+      <c r="V74" t="s">
+        <v>231</v>
+      </c>
+      <c r="X74" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="75" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>113</v>
+      </c>
+      <c r="C75" t="s">
+        <v>414</v>
+      </c>
+      <c r="D75" t="s">
+        <v>404</v>
+      </c>
+      <c r="E75" t="s">
+        <v>397</v>
+      </c>
+      <c r="F75" t="s">
+        <v>137</v>
+      </c>
+      <c r="G75" t="s">
+        <v>238</v>
+      </c>
+      <c r="H75" t="s">
+        <v>265</v>
+      </c>
+      <c r="I75" t="s">
+        <v>240</v>
+      </c>
+      <c r="J75" t="s">
+        <v>222</v>
+      </c>
+      <c r="K75" t="s">
+        <v>155</v>
+      </c>
+      <c r="L75" t="s">
+        <v>35</v>
+      </c>
+      <c r="M75" t="s">
+        <v>35</v>
+      </c>
+      <c r="N75" t="s">
+        <v>36</v>
+      </c>
+      <c r="O75" t="s">
+        <v>37</v>
+      </c>
+      <c r="P75" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q75" t="s">
+        <v>38</v>
+      </c>
+      <c r="R75" t="s">
+        <v>390</v>
+      </c>
+      <c r="S75" t="s">
+        <v>269</v>
+      </c>
+      <c r="T75" t="s">
+        <v>271</v>
+      </c>
+      <c r="U75" t="s">
+        <v>381</v>
+      </c>
+      <c r="V75" t="s">
+        <v>231</v>
+      </c>
+      <c r="X75" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="76" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>113</v>
+      </c>
+      <c r="C76" t="s">
+        <v>413</v>
+      </c>
+      <c r="D76" t="s">
+        <v>403</v>
+      </c>
+      <c r="E76" t="s">
+        <v>344</v>
+      </c>
+      <c r="F76" t="s">
+        <v>137</v>
+      </c>
+      <c r="G76" t="s">
+        <v>238</v>
+      </c>
+      <c r="H76" t="s">
+        <v>244</v>
+      </c>
+      <c r="I76" t="s">
+        <v>240</v>
+      </c>
+      <c r="J76" t="s">
+        <v>222</v>
+      </c>
+      <c r="K76" t="s">
+        <v>155</v>
+      </c>
+      <c r="L76" t="s">
+        <v>35</v>
+      </c>
+      <c r="M76" t="s">
+        <v>35</v>
+      </c>
+      <c r="N76" t="s">
+        <v>36</v>
+      </c>
+      <c r="O76" t="s">
+        <v>37</v>
+      </c>
+      <c r="P76" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q76" t="s">
+        <v>38</v>
+      </c>
+      <c r="R76" t="s">
+        <v>393</v>
+      </c>
+      <c r="S76" t="s">
+        <v>269</v>
+      </c>
+      <c r="T76" t="s">
+        <v>387</v>
+      </c>
+      <c r="U76" t="s">
+        <v>381</v>
+      </c>
+      <c r="V76" t="s">
+        <v>231</v>
+      </c>
+      <c r="X76" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="77" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>113</v>
+      </c>
+      <c r="C77" t="s">
+        <v>412</v>
+      </c>
+      <c r="D77" t="s">
+        <v>402</v>
+      </c>
+      <c r="E77" t="s">
+        <v>396</v>
+      </c>
+      <c r="F77" t="s">
+        <v>263</v>
+      </c>
+      <c r="G77" t="s">
+        <v>238</v>
+      </c>
+      <c r="H77" t="s">
+        <v>244</v>
+      </c>
+      <c r="I77" t="s">
+        <v>240</v>
+      </c>
+      <c r="J77" t="s">
+        <v>222</v>
+      </c>
+      <c r="K77" t="s">
+        <v>155</v>
+      </c>
+      <c r="L77" t="s">
+        <v>35</v>
+      </c>
+      <c r="M77" t="s">
+        <v>35</v>
+      </c>
+      <c r="N77" t="s">
+        <v>36</v>
+      </c>
+      <c r="O77" t="s">
+        <v>37</v>
+      </c>
+      <c r="P77" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>38</v>
+      </c>
+      <c r="R77" t="s">
+        <v>392</v>
+      </c>
+      <c r="S77" t="s">
+        <v>388</v>
+      </c>
+      <c r="T77" t="s">
+        <v>386</v>
+      </c>
+      <c r="U77" t="s">
+        <v>382</v>
+      </c>
+      <c r="V77" t="s">
+        <v>273</v>
+      </c>
+      <c r="X77" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="78" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>113</v>
+      </c>
+      <c r="C78" t="s">
+        <v>411</v>
+      </c>
+      <c r="D78" t="s">
+        <v>401</v>
+      </c>
+      <c r="E78" t="s">
+        <v>396</v>
+      </c>
+      <c r="F78" t="s">
+        <v>263</v>
+      </c>
+      <c r="G78" t="s">
+        <v>238</v>
+      </c>
+      <c r="H78" t="s">
+        <v>244</v>
+      </c>
+      <c r="I78" t="s">
+        <v>240</v>
+      </c>
+      <c r="J78" t="s">
+        <v>222</v>
+      </c>
+      <c r="K78" t="s">
+        <v>155</v>
+      </c>
+      <c r="L78" t="s">
+        <v>35</v>
+      </c>
+      <c r="M78" t="s">
+        <v>35</v>
+      </c>
+      <c r="N78" t="s">
+        <v>36</v>
+      </c>
+      <c r="O78" t="s">
+        <v>37</v>
+      </c>
+      <c r="P78" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>38</v>
+      </c>
+      <c r="R78" t="s">
+        <v>391</v>
+      </c>
+      <c r="S78" t="s">
+        <v>269</v>
+      </c>
+      <c r="T78" t="s">
+        <v>385</v>
+      </c>
+      <c r="U78" t="s">
+        <v>229</v>
+      </c>
+      <c r="V78" t="s">
+        <v>273</v>
+      </c>
+      <c r="X78" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="79" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>113</v>
+      </c>
+      <c r="C79" t="s">
+        <v>410</v>
+      </c>
+      <c r="D79" t="s">
+        <v>400</v>
+      </c>
+      <c r="E79" t="s">
+        <v>154</v>
+      </c>
+      <c r="F79" t="s">
+        <v>263</v>
+      </c>
+      <c r="G79" t="s">
+        <v>238</v>
+      </c>
+      <c r="H79" t="s">
+        <v>395</v>
+      </c>
+      <c r="I79" t="s">
+        <v>240</v>
+      </c>
+      <c r="J79" t="s">
+        <v>222</v>
+      </c>
+      <c r="K79" t="s">
+        <v>155</v>
+      </c>
+      <c r="L79" t="s">
+        <v>35</v>
+      </c>
+      <c r="M79" t="s">
+        <v>35</v>
+      </c>
+      <c r="N79" t="s">
+        <v>36</v>
+      </c>
+      <c r="O79" t="s">
+        <v>37</v>
+      </c>
+      <c r="P79" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q79" t="s">
+        <v>38</v>
+      </c>
+      <c r="R79" t="s">
+        <v>390</v>
+      </c>
+      <c r="S79" t="s">
+        <v>269</v>
+      </c>
+      <c r="T79" t="s">
+        <v>271</v>
+      </c>
+      <c r="U79" t="s">
+        <v>381</v>
+      </c>
+      <c r="V79" t="s">
+        <v>231</v>
+      </c>
+      <c r="X79" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="80" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>113</v>
+      </c>
+      <c r="C80" t="s">
+        <v>409</v>
+      </c>
+      <c r="D80" t="s">
+        <v>399</v>
+      </c>
+      <c r="E80" t="s">
+        <v>280</v>
+      </c>
+      <c r="F80" t="s">
+        <v>285</v>
+      </c>
+      <c r="G80" t="s">
+        <v>238</v>
+      </c>
+      <c r="H80" t="s">
+        <v>395</v>
+      </c>
+      <c r="I80" t="s">
+        <v>240</v>
+      </c>
+      <c r="J80" t="s">
+        <v>222</v>
+      </c>
+      <c r="K80" t="s">
+        <v>155</v>
+      </c>
+      <c r="L80" t="s">
+        <v>35</v>
+      </c>
+      <c r="M80" t="s">
+        <v>35</v>
+      </c>
+      <c r="N80" t="s">
+        <v>36</v>
+      </c>
+      <c r="O80" t="s">
+        <v>37</v>
+      </c>
+      <c r="P80" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q80" t="s">
+        <v>38</v>
+      </c>
+      <c r="R80" t="s">
+        <v>390</v>
+      </c>
+      <c r="S80" t="s">
+        <v>269</v>
+      </c>
+      <c r="T80" t="s">
+        <v>271</v>
+      </c>
+      <c r="U80" t="s">
+        <v>381</v>
+      </c>
+      <c r="V80" t="s">
+        <v>231</v>
+      </c>
+      <c r="X80" t="s">
+        <v>399</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Allows query for new configs
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noahd\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F0062E-BDBD-4390-BC93-E91D92A5B7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB96CB3-72B0-4C9E-80B1-375C3AB6DE36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3750" yWindow="4095" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2004" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2010" uniqueCount="394">
   <si>
     <t>make</t>
   </si>
@@ -453,12 +453,6 @@
   </si>
   <si>
     <t>radeon graphics</t>
-  </si>
-  <si>
-    <t>z13</t>
-  </si>
-  <si>
-    <t>t14 g1 amd</t>
   </si>
   <si>
     <t>lenovo</t>
@@ -1575,8 +1569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="X90" sqref="X90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1669,13 +1663,13 @@
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>25</v>
@@ -1746,13 +1740,13 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>25</v>
@@ -1823,13 +1817,13 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>42</v>
@@ -1856,16 +1850,16 @@
         <v>46</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>99</v>
@@ -1900,13 +1894,13 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>51</v>
@@ -1933,13 +1927,13 @@
         <v>31</v>
       </c>
       <c r="L5" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>155</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>138</v>
@@ -1977,13 +1971,13 @@
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>57</v>
@@ -2054,13 +2048,13 @@
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>59</v>
@@ -2131,13 +2125,13 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>63</v>
@@ -2208,13 +2202,13 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>66</v>
@@ -2285,16 +2279,16 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>69</v>
@@ -2354,7 +2348,7 @@
         <v>37</v>
       </c>
       <c r="X10" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="Y10" s="1" t="s">
         <v>65</v>
@@ -2362,16 +2356,16 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>71</v>
@@ -2431,7 +2425,7 @@
         <v>37</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="Y11" s="1" t="s">
         <v>65</v>
@@ -2439,13 +2433,13 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>130</v>
@@ -2508,7 +2502,7 @@
         <v>37</v>
       </c>
       <c r="X12" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="Y12" s="1" t="s">
         <v>65</v>
@@ -2516,13 +2510,13 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>66</v>
@@ -2593,13 +2587,13 @@
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>130</v>
@@ -2662,7 +2656,7 @@
         <v>37</v>
       </c>
       <c r="X14" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="Y14" s="1" t="s">
         <v>74</v>
@@ -2670,13 +2664,13 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>63</v>
@@ -2750,13 +2744,13 @@
         <v>88</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>178</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>69</v>
@@ -2816,7 +2810,7 @@
         <v>37</v>
       </c>
       <c r="X16" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="Y16" s="2">
         <v>2141</v>
@@ -2827,13 +2821,13 @@
         <v>88</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>83</v>
@@ -2893,7 +2887,7 @@
         <v>37</v>
       </c>
       <c r="X17" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="Y17" s="2">
         <v>2141</v>
@@ -2904,13 +2898,13 @@
         <v>88</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>83</v>
@@ -2970,7 +2964,7 @@
         <v>37</v>
       </c>
       <c r="X18" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="Y18" s="2">
         <v>2141</v>
@@ -2981,13 +2975,13 @@
         <v>88</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>111</v>
@@ -3005,7 +2999,7 @@
         <v>30</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>31</v>
@@ -3047,10 +3041,10 @@
         <v>37</v>
       </c>
       <c r="X19" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="Y19" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
@@ -3058,13 +3052,13 @@
         <v>88</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>111</v>
@@ -3082,7 +3076,7 @@
         <v>30</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>31</v>
@@ -3109,7 +3103,7 @@
         <v>89</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="T20" s="1" t="s">
         <v>90</v>
@@ -3124,10 +3118,10 @@
         <v>37</v>
       </c>
       <c r="X20" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="Y20" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
@@ -3135,13 +3129,13 @@
         <v>88</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>111</v>
@@ -3159,7 +3153,7 @@
         <v>30</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>31</v>
@@ -3186,7 +3180,7 @@
         <v>89</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="T21" s="1" t="s">
         <v>90</v>
@@ -3201,10 +3195,10 @@
         <v>37</v>
       </c>
       <c r="X21" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="Y21" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
@@ -3212,13 +3206,13 @@
         <v>88</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>185</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>111</v>
@@ -3236,7 +3230,7 @@
         <v>30</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>31</v>
@@ -3278,21 +3272,21 @@
         <v>37</v>
       </c>
       <c r="X22" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="Y22" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>92</v>
@@ -3363,7 +3357,7 @@
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>100</v>
@@ -3440,7 +3434,7 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>104</v>
@@ -3517,13 +3511,13 @@
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>106</v>
@@ -3594,13 +3588,13 @@
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>109</v>
@@ -3671,13 +3665,13 @@
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>113</v>
@@ -3748,13 +3742,13 @@
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>117</v>
@@ -3825,13 +3819,13 @@
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>211</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>117</v>
@@ -3905,28 +3899,28 @@
         <v>88</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="G31" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="H31" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="I31" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>219</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>97</v>
@@ -3953,10 +3947,10 @@
         <v>88</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="S31" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="T31" s="1" t="s">
         <v>122</v>
@@ -3971,7 +3965,7 @@
         <v>37</v>
       </c>
       <c r="X31" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
@@ -3979,31 +3973,31 @@
         <v>88</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="F32" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="H32" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="F32" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="G32" s="1" t="s">
+      <c r="I32" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="H32" s="1" t="s">
+      <c r="J32" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>97</v>
@@ -4027,25 +4021,25 @@
         <v>88</v>
       </c>
       <c r="R32" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="S32" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="T32" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="U32" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="S32" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="T32" s="1" t="s">
+      <c r="V32" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="U32" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="V32" s="1" t="s">
-        <v>234</v>
       </c>
       <c r="W32" s="1" t="s">
         <v>37</v>
       </c>
       <c r="X32" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
@@ -4053,16 +4047,16 @@
         <v>88</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>239</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>40</v>
@@ -4101,7 +4095,7 @@
         <v>88</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="S33" s="1" t="s">
         <v>40</v>
@@ -4124,28 +4118,28 @@
         <v>88</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="E34" s="1" t="s">
+      <c r="G34" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H34" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="G34" s="1" t="s">
+      <c r="I34" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="H34" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>229</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>97</v>
@@ -4172,16 +4166,16 @@
         <v>88</v>
       </c>
       <c r="R34" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="S34" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="T34" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="S34" s="1" t="s">
+      <c r="U34" s="1" t="s">
         <v>247</v>
-      </c>
-      <c r="T34" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="U34" s="1" t="s">
-        <v>249</v>
       </c>
       <c r="V34" s="1" t="s">
         <v>82</v>
@@ -4192,13 +4186,13 @@
         <v>88</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>252</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>83</v>
@@ -4240,25 +4234,25 @@
         <v>32</v>
       </c>
       <c r="R35" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="S35" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="T35" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="S35" s="1" t="s">
+      <c r="U35" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="T35" s="1" t="s">
+      <c r="V35" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="U35" s="1" t="s">
+      <c r="W35" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="V35" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="W35" s="1" t="s">
-        <v>258</v>
-      </c>
       <c r="X35" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
@@ -4266,19 +4260,19 @@
         <v>88</v>
       </c>
       <c r="C36" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E36" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>261</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>27</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>29</v>
@@ -4311,10 +4305,10 @@
         <v>32</v>
       </c>
       <c r="R36" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="S36" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="T36" s="1" t="s">
         <v>124</v>
@@ -4326,7 +4320,7 @@
         <v>82</v>
       </c>
       <c r="X36" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
@@ -4334,7 +4328,7 @@
         <v>88</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>105</v>
@@ -4391,10 +4385,10 @@
         <v>81</v>
       </c>
       <c r="V37" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="W37" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="X37" s="1" t="s">
         <v>105</v>
@@ -4405,10 +4399,10 @@
         <v>88</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>83</v>
@@ -4462,13 +4456,13 @@
         <v>81</v>
       </c>
       <c r="V38" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="W38" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="X38" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
@@ -4476,10 +4470,10 @@
         <v>88</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>83</v>
@@ -4491,7 +4485,7 @@
         <v>28</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>30</v>
@@ -4536,10 +4530,10 @@
         <v>82</v>
       </c>
       <c r="W39" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="X39" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
@@ -4547,13 +4541,13 @@
         <v>88</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>272</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>40</v>
@@ -4592,25 +4586,25 @@
         <v>32</v>
       </c>
       <c r="R40" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="S40" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="T40" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="S40" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="T40" s="1" t="s">
+      <c r="U40" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="V40" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="U40" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="V40" s="1" t="s">
-        <v>257</v>
-      </c>
       <c r="W40" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="X40" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
@@ -4618,7 +4612,7 @@
         <v>88</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>105</v>
@@ -4663,19 +4657,19 @@
         <v>77</v>
       </c>
       <c r="R41" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="S41" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="T41" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="S41" s="1" t="s">
+      <c r="U41" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="T41" s="1" t="s">
+      <c r="V41" s="1" t="s">
         <v>278</v>
-      </c>
-      <c r="U41" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="V41" s="1" t="s">
-        <v>280</v>
       </c>
       <c r="X41" s="1" t="s">
         <v>105</v>
@@ -4686,10 +4680,10 @@
         <v>88</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>52</v>
@@ -4707,7 +4701,7 @@
         <v>30</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>97</v>
@@ -4731,22 +4725,22 @@
         <v>32</v>
       </c>
       <c r="R42" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="S42" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="T42" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="U42" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="V42" s="1" t="s">
         <v>82</v>
       </c>
       <c r="X42" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
@@ -4754,10 +4748,10 @@
         <v>88</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>52</v>
@@ -4799,25 +4793,25 @@
         <v>32</v>
       </c>
       <c r="R43" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="S43" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="T43" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="U43" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="V43" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="W43" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="S43" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="T43" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="U43" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="V43" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="W43" s="1" t="s">
-        <v>286</v>
-      </c>
       <c r="X43" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.25">
@@ -4825,10 +4819,10 @@
         <v>88</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>137</v>
@@ -4870,25 +4864,25 @@
         <v>32</v>
       </c>
       <c r="R44" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="S44" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="T44" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="U44" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="S44" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="T44" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="U44" s="1" t="s">
-        <v>291</v>
-      </c>
       <c r="V44" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="W44" s="1" t="s">
         <v>127</v>
       </c>
       <c r="X44" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.25">
@@ -4896,10 +4890,10 @@
         <v>88</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>72</v>
@@ -4941,22 +4935,22 @@
         <v>32</v>
       </c>
       <c r="R45" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="S45" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="T45" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="U45" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="S45" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="T45" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="U45" s="1" t="s">
+      <c r="V45" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="X45" s="1" t="s">
         <v>291</v>
-      </c>
-      <c r="V45" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="X45" s="1" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.25">
@@ -4964,10 +4958,10 @@
         <v>88</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>72</v>
@@ -5009,10 +5003,10 @@
         <v>32</v>
       </c>
       <c r="R46" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="S46" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="T46" s="1" t="s">
         <v>124</v>
@@ -5024,7 +5018,7 @@
         <v>82</v>
       </c>
       <c r="X46" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.25">
@@ -5032,10 +5026,10 @@
         <v>88</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>83</v>
@@ -5077,22 +5071,22 @@
         <v>77</v>
       </c>
       <c r="R47" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="S47" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="T47" s="1" t="s">
         <v>125</v>
       </c>
       <c r="U47" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="V47" s="1" t="s">
         <v>82</v>
       </c>
       <c r="X47" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.25">
@@ -5100,10 +5094,10 @@
         <v>88</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>83</v>
@@ -5145,7 +5139,7 @@
         <v>77</v>
       </c>
       <c r="R48" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="S48" s="1" t="s">
         <v>79</v>
@@ -5160,7 +5154,7 @@
         <v>82</v>
       </c>
       <c r="X48" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.25">
@@ -5168,7 +5162,7 @@
         <v>88</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>101</v>
@@ -5213,19 +5207,19 @@
         <v>77</v>
       </c>
       <c r="R49" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="S49" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="T49" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="S49" s="1" t="s">
+      <c r="U49" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="T49" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="U49" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="V49" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="W49" s="1" t="s">
         <v>126</v>
@@ -5239,7 +5233,7 @@
         <v>88</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>101</v>
@@ -5284,19 +5278,19 @@
         <v>77</v>
       </c>
       <c r="R50" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="S50" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="T50" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="S50" s="1" t="s">
+      <c r="U50" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="T50" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="U50" s="1" t="s">
-        <v>279</v>
-      </c>
       <c r="V50" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="W50" s="1" t="s">
         <v>126</v>
@@ -5310,10 +5304,10 @@
         <v>88</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>52</v>
@@ -5355,22 +5349,22 @@
         <v>32</v>
       </c>
       <c r="R51" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="S51" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="T51" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="U51" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="V51" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="U51" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="V51" s="1" t="s">
-        <v>257</v>
-      </c>
       <c r="X51" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.25">
@@ -5378,10 +5372,10 @@
         <v>88</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>83</v>
@@ -5423,22 +5417,22 @@
         <v>32</v>
       </c>
       <c r="R52" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="S52" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="T52" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="U52" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="S52" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="T52" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="U52" s="1" t="s">
-        <v>291</v>
-      </c>
       <c r="V52" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="X52" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.25">
@@ -5446,10 +5440,10 @@
         <v>88</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>137</v>
@@ -5491,25 +5485,25 @@
         <v>32</v>
       </c>
       <c r="R53" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="S53" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="T53" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="U53" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="S53" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="T53" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="U53" s="1" t="s">
-        <v>291</v>
-      </c>
       <c r="V53" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="W53" s="1" t="s">
         <v>127</v>
       </c>
       <c r="X53" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.25">
@@ -5517,13 +5511,13 @@
         <v>88</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>304</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>306</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>40</v>
@@ -5562,22 +5556,22 @@
         <v>77</v>
       </c>
       <c r="R54" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="S54" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="T54" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="S54" s="1" t="s">
+      <c r="U54" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="T54" s="1" t="s">
+      <c r="V54" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="U54" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="V54" s="1" t="s">
-        <v>280</v>
-      </c>
       <c r="X54" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.25">
@@ -5585,16 +5579,16 @@
         <v>88</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E55" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="F55" s="1" t="s">
         <v>306</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>308</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>28</v>
@@ -5630,22 +5624,22 @@
         <v>77</v>
       </c>
       <c r="R55" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="S55" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="T55" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="S55" s="1" t="s">
+      <c r="U55" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="T55" s="1" t="s">
+      <c r="V55" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="U55" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="V55" s="1" t="s">
-        <v>280</v>
-      </c>
       <c r="X55" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.25">
@@ -5653,13 +5647,13 @@
         <v>88</v>
       </c>
       <c r="C56" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>309</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>311</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>40</v>
@@ -5698,10 +5692,10 @@
         <v>32</v>
       </c>
       <c r="R56" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="S56" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="T56" s="1" t="s">
         <v>124</v>
@@ -5713,7 +5707,7 @@
         <v>82</v>
       </c>
       <c r="X56" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.25">
@@ -5721,10 +5715,10 @@
         <v>88</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>137</v>
@@ -5766,25 +5760,25 @@
         <v>77</v>
       </c>
       <c r="R57" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="S57" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="T57" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="S57" s="1" t="s">
+      <c r="U57" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="V57" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="W57" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="T57" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="U57" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="V57" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="W57" s="1" t="s">
-        <v>318</v>
-      </c>
       <c r="X57" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.25">
@@ -5792,13 +5786,13 @@
         <v>88</v>
       </c>
       <c r="C58" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E58" s="1" t="s">
         <v>319</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>321</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>27</v>
@@ -5837,10 +5831,10 @@
         <v>32</v>
       </c>
       <c r="R58" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="S58" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="T58" s="1" t="s">
         <v>124</v>
@@ -5852,7 +5846,7 @@
         <v>82</v>
       </c>
       <c r="X58" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.25">
@@ -5860,13 +5854,13 @@
         <v>88</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="E59" s="1" t="s">
         <v>323</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>325</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>40</v>
@@ -5905,7 +5899,7 @@
         <v>77</v>
       </c>
       <c r="R59" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="S59" s="1" t="s">
         <v>79</v>
@@ -5914,13 +5908,13 @@
         <v>125</v>
       </c>
       <c r="U59" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="V59" s="1" t="s">
         <v>82</v>
       </c>
       <c r="X59" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.25">
@@ -5928,13 +5922,13 @@
         <v>88</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>40</v>
@@ -5973,25 +5967,25 @@
         <v>77</v>
       </c>
       <c r="R60" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="S60" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="T60" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="U60" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="V60" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="W60" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="X60" s="1" t="s">
         <v>326</v>
-      </c>
-      <c r="S60" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="T60" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="U60" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="V60" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="W60" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="X60" s="1" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.25">
@@ -5999,13 +5993,13 @@
         <v>88</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>40</v>
@@ -6044,7 +6038,7 @@
         <v>77</v>
       </c>
       <c r="R61" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="S61" s="1" t="s">
         <v>79</v>
@@ -6059,7 +6053,7 @@
         <v>82</v>
       </c>
       <c r="X61" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.25">
@@ -6067,10 +6061,10 @@
         <v>88</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>72</v>
@@ -6112,7 +6106,7 @@
         <v>77</v>
       </c>
       <c r="R62" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="S62" s="1" t="s">
         <v>49</v>
@@ -6124,10 +6118,10 @@
         <v>81</v>
       </c>
       <c r="V62" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="X62" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.25">
@@ -6135,10 +6129,10 @@
         <v>88</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>137</v>
@@ -6180,22 +6174,22 @@
         <v>77</v>
       </c>
       <c r="R63" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="S63" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="T63" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="S63" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="T63" s="1" t="s">
-        <v>317</v>
-      </c>
       <c r="U63" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="V63" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="X63" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="64" spans="1:24" x14ac:dyDescent="0.25">
@@ -6203,13 +6197,13 @@
         <v>88</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>27</v>
@@ -6248,25 +6242,25 @@
         <v>32</v>
       </c>
       <c r="R64" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="S64" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="T64" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="U64" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="T64" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="U64" s="1" t="s">
-        <v>256</v>
-      </c>
       <c r="V64" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="W64" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="X64" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="65" spans="1:24" x14ac:dyDescent="0.25">
@@ -6274,13 +6268,13 @@
         <v>88</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="E65" s="1" t="s">
         <v>342</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>344</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>40</v>
@@ -6289,7 +6283,7 @@
         <v>28</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="I65" s="1" t="s">
         <v>30</v>
@@ -6319,25 +6313,25 @@
         <v>32</v>
       </c>
       <c r="R65" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="S65" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="T65" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="U65" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="V65" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="W65" s="1" t="s">
         <v>128</v>
       </c>
       <c r="X65" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="66" spans="1:24" x14ac:dyDescent="0.25">
@@ -6345,13 +6339,13 @@
         <v>88</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>40</v>
@@ -6390,22 +6384,22 @@
         <v>77</v>
       </c>
       <c r="R66" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="S66" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="T66" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="U66" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="V66" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="X66" s="1" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="67" spans="1:24" x14ac:dyDescent="0.25">
@@ -6413,13 +6407,13 @@
         <v>88</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>27</v>
@@ -6458,25 +6452,25 @@
         <v>32</v>
       </c>
       <c r="R67" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="S67" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="T67" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="U67" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="T67" s="1" t="s">
+      <c r="V67" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="U67" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="V67" s="1" t="s">
-        <v>257</v>
-      </c>
       <c r="W67" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="X67" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="68" spans="1:24" x14ac:dyDescent="0.25">
@@ -6484,13 +6478,13 @@
         <v>88</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>27</v>
@@ -6529,10 +6523,10 @@
         <v>32</v>
       </c>
       <c r="R68" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="S68" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="T68" s="1" t="s">
         <v>124</v>
@@ -6544,7 +6538,7 @@
         <v>82</v>
       </c>
       <c r="X68" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="69" spans="1:24" x14ac:dyDescent="0.25">
@@ -6552,10 +6546,10 @@
         <v>88</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>137</v>
@@ -6597,25 +6591,25 @@
         <v>32</v>
       </c>
       <c r="R69" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="S69" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="T69" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="U69" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="V69" s="1" t="s">
         <v>82</v>
       </c>
       <c r="W69" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="X69" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="70" spans="1:24" x14ac:dyDescent="0.25">
@@ -6623,10 +6617,10 @@
         <v>88</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>137</v>
@@ -6668,25 +6662,25 @@
         <v>32</v>
       </c>
       <c r="R70" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="S70" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="T70" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="U70" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="V70" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="W70" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="S70" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="T70" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="U70" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="V70" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="W70" s="1" t="s">
+      <c r="X70" s="1" t="s">
         <v>355</v>
-      </c>
-      <c r="X70" s="1" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="71" spans="1:24" x14ac:dyDescent="0.25">
@@ -6694,13 +6688,13 @@
         <v>88</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>27</v>
@@ -6739,25 +6733,25 @@
         <v>32</v>
       </c>
       <c r="R71" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="S71" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="T71" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="U71" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="V71" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="W71" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="S71" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="T71" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="U71" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="V71" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="W71" s="1" t="s">
-        <v>355</v>
-      </c>
       <c r="X71" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="72" spans="1:24" x14ac:dyDescent="0.25">
@@ -6765,13 +6759,13 @@
         <v>88</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>40</v>
@@ -6810,10 +6804,10 @@
         <v>32</v>
       </c>
       <c r="R72" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="S72" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="T72" s="1" t="s">
         <v>124</v>
@@ -6825,7 +6819,7 @@
         <v>82</v>
       </c>
       <c r="X72" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="73" spans="1:24" x14ac:dyDescent="0.25">
@@ -6833,10 +6827,10 @@
         <v>88</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>71</v>
@@ -6878,25 +6872,25 @@
         <v>32</v>
       </c>
       <c r="R73" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="S73" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="T73" s="1" t="s">
         <v>124</v>
       </c>
       <c r="U73" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="V73" s="1" t="s">
         <v>82</v>
       </c>
       <c r="W73" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="X73" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="74" spans="1:24" x14ac:dyDescent="0.25">
@@ -6904,10 +6898,10 @@
         <v>88</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>72</v>
@@ -6949,10 +6943,10 @@
         <v>32</v>
       </c>
       <c r="R74" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="S74" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="T74" s="1" t="s">
         <v>124</v>
@@ -6964,7 +6958,7 @@
         <v>82</v>
       </c>
       <c r="X74" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="75" spans="1:24" x14ac:dyDescent="0.25">
@@ -6972,13 +6966,13 @@
         <v>88</v>
       </c>
       <c r="C75" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="E75" s="1" t="s">
         <v>371</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>373</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>40</v>
@@ -7017,10 +7011,10 @@
         <v>32</v>
       </c>
       <c r="R75" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="S75" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="T75" s="1" t="s">
         <v>124</v>
@@ -7032,7 +7026,7 @@
         <v>82</v>
       </c>
       <c r="X75" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="76" spans="1:24" x14ac:dyDescent="0.25">
@@ -7040,13 +7034,13 @@
         <v>88</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>40</v>
@@ -7085,10 +7079,10 @@
         <v>32</v>
       </c>
       <c r="R76" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="S76" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="T76" s="1" t="s">
         <v>124</v>
@@ -7100,7 +7094,7 @@
         <v>82</v>
       </c>
       <c r="X76" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="77" spans="1:24" x14ac:dyDescent="0.25">
@@ -7108,13 +7102,13 @@
         <v>88</v>
       </c>
       <c r="C77" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="E77" s="1" t="s">
         <v>374</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>376</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>27</v>
@@ -7153,22 +7147,22 @@
         <v>32</v>
       </c>
       <c r="R77" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="S77" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="T77" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="S77" s="1" t="s">
+      <c r="U77" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="T77" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="U77" s="1" t="s">
-        <v>380</v>
-      </c>
       <c r="V77" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="X77" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="78" spans="1:24" x14ac:dyDescent="0.25">
@@ -7176,13 +7170,13 @@
         <v>88</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>27</v>
@@ -7221,10 +7215,10 @@
         <v>32</v>
       </c>
       <c r="R78" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="S78" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="T78" s="1" t="s">
         <v>129</v>
@@ -7233,10 +7227,10 @@
         <v>81</v>
       </c>
       <c r="V78" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="X78" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="79" spans="1:24" x14ac:dyDescent="0.25">
@@ -7244,10 +7238,10 @@
         <v>88</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>71</v>
@@ -7259,7 +7253,7 @@
         <v>28</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I79" s="1" t="s">
         <v>30</v>
@@ -7289,10 +7283,10 @@
         <v>32</v>
       </c>
       <c r="R79" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="S79" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="T79" s="1" t="s">
         <v>124</v>
@@ -7304,7 +7298,7 @@
         <v>82</v>
       </c>
       <c r="X79" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="80" spans="1:24" x14ac:dyDescent="0.25">
@@ -7312,10 +7306,10 @@
         <v>88</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>69</v>
@@ -7327,7 +7321,7 @@
         <v>28</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I80" s="1" t="s">
         <v>30</v>
@@ -7357,10 +7351,10 @@
         <v>32</v>
       </c>
       <c r="R80" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="S80" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="T80" s="1" t="s">
         <v>124</v>
@@ -7372,15 +7366,18 @@
         <v>82</v>
       </c>
       <c r="X80" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="81" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>386</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>132</v>
@@ -7445,7 +7442,10 @@
     </row>
     <row r="82" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>135</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>135</v>
@@ -7513,10 +7513,13 @@
     </row>
     <row r="83" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>388</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>136</v>
@@ -7581,13 +7584,16 @@
     </row>
     <row r="84" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>389</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>137</v>
@@ -7644,18 +7650,21 @@
         <v>36</v>
       </c>
       <c r="X84" s="1" t="s">
-        <v>140</v>
+        <v>390</v>
       </c>
     </row>
     <row r="85" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>391</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>137</v>
@@ -7712,18 +7721,21 @@
         <v>36</v>
       </c>
       <c r="X85" s="1" t="s">
-        <v>140</v>
+        <v>390</v>
       </c>
     </row>
     <row r="86" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>392</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>26</v>
@@ -7780,7 +7792,7 @@
         <v>36</v>
       </c>
       <c r="X86" s="1" t="s">
-        <v>141</v>
+        <v>393</v>
       </c>
     </row>
   </sheetData>

</xml_diff>